<commit_message>
adjust EFs calcualtions for individual studies
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17DA2F1F-1176-4321-84BC-474ABB99768F}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3074FFDD-5426-4B07-9EA2-FD7110E00061}"/>
   <bookViews>
-    <workbookView xWindow="-1860" yWindow="-18915" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -3016,8 +3016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EFs of ID3: filtered to just include lags 2,3, and 4
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3074FFDD-5426-4B07-9EA2-FD7110E00061}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCE28B44-A3E0-45E8-9F91-3493146621CB}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="260">
   <si>
     <t>CognitiveFunction</t>
   </si>
@@ -1134,24 +1134,6 @@
     <t>attentional blink</t>
   </si>
   <si>
-    <t xml:space="preserve">calculations based on raw data provided.
-mean accuracy Psilocybin: 0.8271889 
-SD accuracy Psilocybin: 0.09645801 
-mean accuracy placebo: 0.8711982  
-SD accuracy placebo: 0.06757419 
-mean RT Psilocybin: 0.8646351  
-SD RT Psilocybin: 0.1826972  
-mean RT placebo: 0.9029352  
-SD RT placebo: 0.2269478  
-</t>
-  </si>
-  <si>
-    <t>-0.1859102</t>
-  </si>
-  <si>
-    <t>-0.5284621</t>
-  </si>
-  <si>
     <t>Incrfeasaed RT for psilo</t>
   </si>
   <si>
@@ -2109,6 +2091,28 @@
   </si>
   <si>
     <t>-1.305</t>
+  </si>
+  <si>
+    <t>-0.4602659</t>
+  </si>
+  <si>
+    <t>-0.2587441</t>
+  </si>
+  <si>
+    <t>we only calcualted the results for lag 2,3 and 4 for RT &amp; ACC.
+RT calcualted for T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calculations based on raw data provided.
+mean accuracy Psilocybin: 0.3520737
+SD accuracy Psilocybin: 0.04880175 
+mean accuracy placebo: 0.371659  
+SD accuracy placebo: 0.03520996  
+mean RT Psilocybin: 0.8614073  
+SD RT Psilocybin: 0.1706961  
+mean RT placebo: 0.9138944 
+SD RT placebo: 0.2353612   
+</t>
   </si>
 </sst>
 </file>
@@ -2653,7 +2657,27 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3016,8 +3040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,13 +3068,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>36</v>
@@ -3225,7 +3249,7 @@
         <v>71</v>
       </c>
       <c r="M4" s="54" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
@@ -3276,7 +3300,7 @@
         <v>75</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -3323,7 +3347,7 @@
         <v>77</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -3370,7 +3394,7 @@
         <v>82</v>
       </c>
       <c r="M7" s="54" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -3387,7 +3411,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>44</v>
@@ -3396,7 +3420,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G8" s="28">
         <v>21</v>
@@ -3405,29 +3429,29 @@
         <v>22</v>
       </c>
       <c r="I8" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="L8" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="N8" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="47" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3438,7 +3462,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>44</v>
@@ -3447,7 +3471,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G9" s="28">
         <v>21</v>
@@ -3456,29 +3480,29 @@
         <v>22</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K9" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="L9" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3489,7 +3513,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>44</v>
@@ -3498,36 +3522,36 @@
         <v>44</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G10" s="28">
         <v>22</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J10" s="28">
         <v>25</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q10" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3538,7 +3562,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>44</v>
@@ -3547,36 +3571,36 @@
         <v>44</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G11" s="28">
         <v>22</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J11" s="28">
         <v>25</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q11" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3661,7 +3685,7 @@
         <v>240</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>68</v>
@@ -3713,7 +3737,7 @@
         <v>79</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
@@ -3749,30 +3773,30 @@
         <v>16</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K15" s="15">
         <v>105</v>
       </c>
       <c r="L15" s="56" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="P15" s="63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q15" s="59" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3813,7 +3837,7 @@
         <v>83</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -3860,7 +3884,7 @@
         <v>88</v>
       </c>
       <c r="M17" s="54" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -3907,7 +3931,7 @@
         <v>89</v>
       </c>
       <c r="M18" s="54" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3955,7 +3979,7 @@
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="54" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="18" t="s">
@@ -4004,7 +4028,7 @@
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="14" t="s">
@@ -4108,7 +4132,7 @@
       <c r="P22" s="18"/>
       <c r="Q22" s="19"/>
     </row>
-    <row r="23" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:17" ht="189" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12">
         <v>3</v>
       </c>
@@ -4142,18 +4166,20 @@
       <c r="K23" s="19">
         <v>180</v>
       </c>
-      <c r="L23" s="17" t="s">
-        <v>111</v>
+      <c r="L23" s="56" t="s">
+        <v>259</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>113</v>
+        <v>256</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="18"/>
-      <c r="Q23" s="19"/>
+      <c r="Q23" s="59" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="24" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12">
@@ -4172,16 +4198,16 @@
         <v>21</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G24" s="15">
         <v>34</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>101</v>
@@ -4190,16 +4216,16 @@
         <v>60</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="18"/>
       <c r="Q24" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4219,16 +4245,16 @@
         <v>11</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G25" s="28">
         <v>16</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I25" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J25" s="28">
         <v>14</v>
@@ -4237,16 +4263,16 @@
         <v>85</v>
       </c>
       <c r="L25" s="47" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="53"/>
       <c r="Q25" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="146.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4266,7 +4292,7 @@
         <v>21</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G26" s="15">
         <v>8</v>
@@ -4275,29 +4301,29 @@
         <v>27</v>
       </c>
       <c r="I26" s="58" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K26" s="15">
         <v>140</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="P26" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q26" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P26" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q26" s="19" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="146.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4317,38 +4343,38 @@
         <v>11</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G27" s="15">
         <v>8</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I27" s="58" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K27" s="15">
         <v>140</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P27" s="52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="146.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4368,16 +4394,16 @@
         <v>11</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G28" s="15">
         <v>8</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I28" s="58" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J28" s="15" t="s">
         <v>28</v>
@@ -4386,20 +4412,20 @@
         <v>140</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P28" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q28" s="59" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4419,7 +4445,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G29" s="15">
         <v>17</v>
@@ -4428,7 +4454,7 @@
         <v>30</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>28</v>
@@ -4437,18 +4463,18 @@
         <v>120</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="18"/>
       <c r="Q29" s="19" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4468,7 +4494,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G30" s="15">
         <v>16</v>
@@ -4480,26 +4506,26 @@
         <v>43</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K30" s="15">
         <v>85</v>
       </c>
       <c r="L30" s="49" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q30" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="353.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4525,30 +4551,30 @@
         <v>16</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I31" s="45" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K31" s="15">
         <v>105</v>
       </c>
       <c r="L31" s="56" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P31" s="62" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4568,36 +4594,36 @@
         <v>11</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G32" s="15">
         <v>12</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K32" s="15">
         <v>100</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="P32" s="43" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4617,36 +4643,36 @@
         <v>11</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G33" s="36">
         <v>12</v>
       </c>
       <c r="H33" s="36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I33" s="46" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J33" s="36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K33" s="36">
         <v>360</v>
       </c>
       <c r="L33" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="P33" s="37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4666,36 +4692,36 @@
         <v>11</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G34" s="21">
         <v>12</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I34" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J34" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K34" s="21">
         <v>100</v>
       </c>
       <c r="L34" s="37" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P34" s="38" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q34" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4715,36 +4741,36 @@
         <v>11</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G35" s="21">
         <v>12</v>
       </c>
       <c r="H35" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J35" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K35" s="21">
         <v>360</v>
       </c>
       <c r="L35" s="37" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P35" s="38" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q35" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4764,35 +4790,35 @@
         <v>21</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G36" s="34">
         <v>40</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I36" s="39" t="s">
         <v>14</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K36" s="34">
         <v>90</v>
       </c>
       <c r="L36" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="Q36" s="34"/>
     </row>
@@ -4817,10 +4843,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I37" s="40" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J37" s="21">
         <v>15</v>
@@ -4829,20 +4855,20 @@
         <v>225</v>
       </c>
       <c r="L37" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="50" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="Q37" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="132" thickBot="1" x14ac:dyDescent="0.45">
@@ -4862,7 +4888,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G38" s="21">
         <v>19</v>
@@ -4871,7 +4897,7 @@
         <v>12</v>
       </c>
       <c r="I38" s="40" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J38" s="21">
         <v>15</v>
@@ -4880,17 +4906,17 @@
         <v>172</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="66" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="Q38" s="34"/>
     </row>
@@ -4911,16 +4937,16 @@
         <v>11</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G39" s="21">
         <v>21</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I39" s="40" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J39" s="21">
         <v>15</v>
@@ -4929,15 +4955,15 @@
         <v>153</v>
       </c>
       <c r="L39" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="Q39" s="34"/>
     </row>
@@ -4958,13 +4984,13 @@
         <v>11</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G40" s="21">
         <v>21</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I40" s="40" t="s">
         <v>14</v>
@@ -4976,10 +5002,10 @@
         <v>166</v>
       </c>
       <c r="L40" s="37" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5068,7 +5094,7 @@
         <v>240</v>
       </c>
       <c r="L42" s="50" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>69</v>
@@ -5150,38 +5176,38 @@
         <v>44</v>
       </c>
       <c r="F44" s="43" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G44" s="44">
         <v>8</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I44" s="40" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K44" s="21">
         <v>140</v>
       </c>
       <c r="L44" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P44" s="50" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q44" s="61" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="353.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -5207,38 +5233,41 @@
         <v>16</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I45" s="65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K45" s="21">
         <v>105</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P45" s="64" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q45" s="61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q45" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
-  <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+  <conditionalFormatting sqref="M1:M22 M24:M1048576">
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M23">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -5265,16 +5294,16 @@
         <v>59</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G1" s="28">
         <v>21</v>
@@ -5283,29 +5312,29 @@
         <v>22</v>
       </c>
       <c r="I1" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="L1" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="N1" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="47" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5316,16 +5345,16 @@
         <v>59</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G2" s="28">
         <v>21</v>
@@ -5334,29 +5363,29 @@
         <v>22</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="K2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Q2" s="28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5367,45 +5396,45 @@
         <v>38</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G3" s="28">
         <v>22</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J3" s="28">
         <v>25</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5416,45 +5445,45 @@
         <v>38</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G4" s="28">
         <v>22</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J4" s="28">
         <v>25</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="Q4" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -5467,8 +5496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,13 +5521,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="60" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F1" s="60" t="s">
         <v>36</v>
@@ -5673,7 +5702,7 @@
         <v>71</v>
       </c>
       <c r="M4" s="54" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
@@ -5724,7 +5753,7 @@
         <v>75</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -5771,7 +5800,7 @@
         <v>77</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -5803,30 +5832,30 @@
         <v>16</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K7" s="15">
         <v>105</v>
       </c>
       <c r="L7" s="56" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="P7" s="63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q7" s="59" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5868,10 +5897,10 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="54" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P8" s="18" t="s">
         <v>93</v>
@@ -5919,7 +5948,7 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="14" t="s">
@@ -6023,7 +6052,7 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="19"/>
     </row>
-    <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -6057,18 +6086,20 @@
       <c r="K12" s="19">
         <v>180</v>
       </c>
-      <c r="L12" s="17" t="s">
-        <v>111</v>
+      <c r="L12" s="56" t="s">
+        <v>259</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>112</v>
+        <v>257</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>113</v>
+        <v>256</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="18"/>
-      <c r="Q12" s="19"/>
+      <c r="Q12" s="59" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12">
@@ -6087,16 +6118,16 @@
         <v>21</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G13" s="15">
         <v>34</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J13" s="15" t="s">
         <v>101</v>
@@ -6105,16 +6136,16 @@
         <v>60</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6134,16 +6165,16 @@
         <v>11</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G14" s="28">
         <v>16</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J14" s="28">
         <v>14</v>
@@ -6152,16 +6183,16 @@
         <v>85</v>
       </c>
       <c r="L14" s="47" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="53"/>
       <c r="Q14" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6181,7 +6212,7 @@
         <v>21</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G15" s="15">
         <v>8</v>
@@ -6190,29 +6221,29 @@
         <v>27</v>
       </c>
       <c r="I15" s="58" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K15" s="15">
         <v>140</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="P15" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q15" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P15" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q15" s="19" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6232,38 +6263,38 @@
         <v>11</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G16" s="15">
         <v>8</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I16" s="58" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K16" s="15">
         <v>140</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P16" s="52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6283,16 +6314,16 @@
         <v>11</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G17" s="15">
         <v>8</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I17" s="58" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>28</v>
@@ -6301,20 +6332,20 @@
         <v>140</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q17" s="59" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6334,7 +6365,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G18" s="15">
         <v>17</v>
@@ -6343,7 +6374,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>28</v>
@@ -6352,18 +6383,18 @@
         <v>120</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="19" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6383,7 +6414,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G19" s="15">
         <v>16</v>
@@ -6395,26 +6426,26 @@
         <v>43</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K19" s="15">
         <v>85</v>
       </c>
       <c r="L19" s="49" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6440,30 +6471,30 @@
         <v>16</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I20" s="45" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K20" s="15">
         <v>105</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P20" s="62" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6483,36 +6514,36 @@
         <v>11</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G21" s="15">
         <v>12</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K21" s="15">
         <v>100</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="P21" s="43" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6532,36 +6563,36 @@
         <v>11</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G22" s="36">
         <v>12</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I22" s="46" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K22" s="36">
         <v>360</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="P22" s="37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6581,36 +6612,36 @@
         <v>11</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G23" s="21">
         <v>12</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K23" s="21">
         <v>100</v>
       </c>
       <c r="L23" s="37" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P23" s="38" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6630,36 +6661,36 @@
         <v>11</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G24" s="21">
         <v>12</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K24" s="21">
         <v>360</v>
       </c>
       <c r="L24" s="37" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P24" s="38" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="Q24" s="21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6679,35 +6710,35 @@
         <v>21</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G25" s="34">
         <v>40</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I25" s="39" t="s">
         <v>14</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K25" s="34">
         <v>90</v>
       </c>
       <c r="L25" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="41" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="Q25" s="34"/>
     </row>
@@ -6732,10 +6763,10 @@
         <v>19</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J26" s="21">
         <v>15</v>
@@ -6744,20 +6775,20 @@
         <v>225</v>
       </c>
       <c r="L26" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="50" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="Q26" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6777,7 +6808,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G27" s="21">
         <v>19</v>
@@ -6786,7 +6817,7 @@
         <v>12</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J27" s="21">
         <v>15</v>
@@ -6795,17 +6826,17 @@
         <v>172</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="66" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="Q27" s="34"/>
     </row>
@@ -6826,16 +6857,16 @@
         <v>11</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G28" s="21">
         <v>21</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I28" s="40" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="J28" s="21">
         <v>15</v>
@@ -6844,15 +6875,15 @@
         <v>153</v>
       </c>
       <c r="L28" s="51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="Q28" s="34"/>
     </row>
@@ -6873,13 +6904,13 @@
         <v>11</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G29" s="21">
         <v>21</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="I29" s="40" t="s">
         <v>14</v>
@@ -6891,10 +6922,10 @@
         <v>166</v>
       </c>
       <c r="L29" s="37" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -6904,16 +6935,16 @@
   </sheetData>
   <autoFilter ref="A1:Q29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="M1 M30:M1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M17 M19:M29">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:N1 M30:N1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6947,13 +6978,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>36</v>
@@ -7030,7 +7061,7 @@
         <v>82</v>
       </c>
       <c r="M2" s="54" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -7121,7 +7152,7 @@
         <v>240</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>68</v>
@@ -7173,7 +7204,7 @@
         <v>79</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
@@ -7224,7 +7255,7 @@
         <v>83</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -7250,38 +7281,38 @@
         <v>44</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G7" s="44">
         <v>8</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K7" s="21">
         <v>140</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P7" s="50" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q7" s="61" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -7307,37 +7338,37 @@
         <v>16</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I8" s="65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K8" s="21">
         <v>105</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P8" s="64" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q8" s="61" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M8">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7365,13 +7396,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>36</v>
@@ -7448,7 +7479,7 @@
         <v>88</v>
       </c>
       <c r="M2" s="54" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -7495,7 +7526,7 @@
         <v>89</v>
       </c>
       <c r="M3" s="54" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -7586,7 +7617,7 @@
         <v>240</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>69</v>
@@ -7653,7 +7684,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M6">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected code for ID(1) - ID(6)
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BF0D65D-DEB3-4A23-A65F-13EBB690C84A}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1706FA1-15EB-4E5C-88D3-929855421817}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2895" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="3840" windowWidth="21600" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="263">
   <si>
     <t>CognitiveFunction</t>
   </si>
@@ -1100,12 +1100,6 @@
 </t>
   </si>
   <si>
-    <t>0.2281833</t>
-  </si>
-  <si>
-    <t>-0.01118468</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 No effect in Go/Nogo between groups</t>
   </si>
@@ -1140,12 +1134,6 @@
     <t>Figure 3F: Part A (median, 1st quartile, 3rd quartile)
 Psilo:   19.83, 17.85, 24.79
 Placebo: 17.52,  16.53, 21.16</t>
-  </si>
-  <si>
-    <t>0.5286334</t>
-  </si>
-  <si>
-    <t>Time to complete in Part A used as RT, as this part captures attention more purely compared to Part B of TMT</t>
   </si>
   <si>
     <t>No significant change</t>
@@ -2109,16 +2097,34 @@
     <t>-0.4025393</t>
   </si>
   <si>
-    <t>only included NOGo trials</t>
-  </si>
-  <si>
-    <t>-0.3069292</t>
-  </si>
-  <si>
     <t>-0.2994538</t>
   </si>
   <si>
-    <t>only included NoGo trials</t>
+    <t>0.7780865</t>
+  </si>
+  <si>
+    <t>-0.1000337</t>
+  </si>
+  <si>
+    <t>only included  incongruent trials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Part B (median, 1st quartile, 3rd quartile)
+# Psilo:   42.13, 36.71, 48.31
+# Placebo: 35.17,  32.08, 45.22</t>
+  </si>
+  <si>
+    <t>Time to complete in Part B used as RT, as this part captures attention more purely compared to Part A of TMT</t>
+  </si>
+  <si>
+    <t>0.7581123</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>only included ACC of NoGo trials</t>
   </si>
 </sst>
 </file>
@@ -2453,7 +2459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2658,12 +2664,38 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3037,7 +3069,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,13 +3096,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>36</v>
@@ -3245,7 +3277,7 @@
         <v>71</v>
       </c>
       <c r="M4" s="54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
@@ -3296,7 +3328,7 @@
         <v>75</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -3343,7 +3375,7 @@
         <v>77</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -3390,7 +3422,7 @@
         <v>82</v>
       </c>
       <c r="M7" s="54" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
@@ -3407,7 +3439,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>44</v>
@@ -3416,7 +3448,7 @@
         <v>44</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G8" s="28">
         <v>21</v>
@@ -3425,29 +3457,29 @@
         <v>22</v>
       </c>
       <c r="I8" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="M8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="47" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q8" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3458,7 +3490,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>44</v>
@@ -3467,7 +3499,7 @@
         <v>44</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G9" s="28">
         <v>21</v>
@@ -3476,29 +3508,29 @@
         <v>22</v>
       </c>
       <c r="I9" s="29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J9" s="28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K9" s="30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Q9" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3509,7 +3541,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>44</v>
@@ -3518,36 +3550,36 @@
         <v>44</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G10" s="28">
         <v>22</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I10" s="29" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J10" s="28">
         <v>25</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="47" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q10" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3558,7 +3590,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D11" s="28" t="s">
         <v>44</v>
@@ -3567,36 +3599,36 @@
         <v>44</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G11" s="28">
         <v>22</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J11" s="28">
         <v>25</v>
       </c>
       <c r="K11" s="30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="47" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q11" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3681,7 +3713,7 @@
         <v>240</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>68</v>
@@ -3733,7 +3765,7 @@
         <v>79</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
@@ -3769,30 +3801,30 @@
         <v>16</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K15" s="15">
         <v>105</v>
       </c>
       <c r="L15" s="56" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P15" s="63" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q15" s="59" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -3833,7 +3865,7 @@
         <v>83</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -3880,7 +3912,7 @@
         <v>88</v>
       </c>
       <c r="M17" s="54" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
@@ -3927,7 +3959,7 @@
         <v>89</v>
       </c>
       <c r="M18" s="54" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3975,7 +4007,7 @@
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="54" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="18" t="s">
@@ -4024,7 +4056,7 @@
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="14" t="s">
@@ -4072,14 +4104,16 @@
         <v>102</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>103</v>
+        <v>255</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="18"/>
-      <c r="Q21" s="19"/>
+      <c r="Q21" s="19" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="22" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
@@ -4098,7 +4132,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G22" s="15">
         <v>34</v>
@@ -4116,18 +4150,16 @@
         <v>150</v>
       </c>
       <c r="L22" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>259</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="M22" s="2"/>
       <c r="N22" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="18"/>
       <c r="Q22" s="19" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="189" thickBot="1" x14ac:dyDescent="0.45">
@@ -4147,13 +4179,13 @@
         <v>21</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G23" s="15">
         <v>34</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I23" s="16" t="s">
         <v>43</v>
@@ -4165,21 +4197,21 @@
         <v>180</v>
       </c>
       <c r="L23" s="56" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="59" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="63" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12">
         <v>3</v>
       </c>
@@ -4196,16 +4228,16 @@
         <v>21</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G24" s="15">
         <v>34</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>101</v>
@@ -4213,17 +4245,19 @@
       <c r="K24" s="19">
         <v>60</v>
       </c>
-      <c r="L24" s="22" t="s">
-        <v>112</v>
+      <c r="L24" s="70" t="s">
+        <v>258</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>113</v>
+        <v>260</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="18"/>
+      <c r="P24" s="71" t="s">
+        <v>110</v>
+      </c>
       <c r="Q24" s="19" t="s">
-        <v>114</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4243,16 +4277,16 @@
         <v>11</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G25" s="28">
         <v>16</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I25" s="28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J25" s="28">
         <v>14</v>
@@ -4261,16 +4295,16 @@
         <v>85</v>
       </c>
       <c r="L25" s="47" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="53"/>
       <c r="Q25" s="28" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="146.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4290,7 +4324,7 @@
         <v>21</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G26" s="15">
         <v>8</v>
@@ -4299,29 +4333,29 @@
         <v>27</v>
       </c>
       <c r="I26" s="58" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K26" s="15">
         <v>140</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="P26" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="146.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4341,38 +4375,38 @@
         <v>11</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G27" s="15">
         <v>8</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I27" s="58" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K27" s="15">
         <v>140</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P27" s="52" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q27" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="146.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4392,16 +4426,16 @@
         <v>11</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G28" s="15">
         <v>8</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I28" s="58" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J28" s="15" t="s">
         <v>28</v>
@@ -4410,20 +4444,20 @@
         <v>140</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="P28" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q28" s="59" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4443,7 +4477,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G29" s="15">
         <v>17</v>
@@ -4452,7 +4486,7 @@
         <v>30</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J29" s="15" t="s">
         <v>28</v>
@@ -4461,18 +4495,18 @@
         <v>120</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="18"/>
       <c r="Q29" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4492,7 +4526,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G30" s="15">
         <v>16</v>
@@ -4504,26 +4538,26 @@
         <v>43</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K30" s="15">
         <v>85</v>
       </c>
       <c r="L30" s="49" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="Q30" s="19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="353.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -4549,30 +4583,30 @@
         <v>16</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I31" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K31" s="15">
         <v>105</v>
       </c>
       <c r="L31" s="56" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P31" s="62" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q31" s="19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4592,36 +4626,36 @@
         <v>11</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G32" s="15">
         <v>12</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K32" s="15">
         <v>100</v>
       </c>
       <c r="L32" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="P32" s="43" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q32" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4641,36 +4675,36 @@
         <v>11</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G33" s="36">
         <v>12</v>
       </c>
       <c r="H33" s="36" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I33" s="46" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J33" s="36" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K33" s="36">
         <v>360</v>
       </c>
       <c r="L33" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="P33" s="37" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q33" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4690,36 +4724,36 @@
         <v>11</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G34" s="21">
         <v>12</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I34" s="40" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J34" s="21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K34" s="21">
         <v>100</v>
       </c>
       <c r="L34" s="37" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="P34" s="38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q34" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4739,36 +4773,36 @@
         <v>11</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G35" s="21">
         <v>12</v>
       </c>
       <c r="H35" s="21" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I35" s="40" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J35" s="21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K35" s="21">
         <v>360</v>
       </c>
       <c r="L35" s="37" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="P35" s="38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q35" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -4788,35 +4822,35 @@
         <v>21</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G36" s="34">
         <v>40</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I36" s="39" t="s">
         <v>14</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K36" s="34">
         <v>90</v>
       </c>
       <c r="L36" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" s="41" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="Q36" s="34"/>
     </row>
@@ -4841,10 +4875,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="21" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I37" s="40" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J37" s="21">
         <v>15</v>
@@ -4853,20 +4887,20 @@
         <v>225</v>
       </c>
       <c r="L37" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="50" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="Q37" s="21" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" spans="1:17" ht="132" thickBot="1" x14ac:dyDescent="0.45">
@@ -4886,7 +4920,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G38" s="21">
         <v>19</v>
@@ -4895,7 +4929,7 @@
         <v>12</v>
       </c>
       <c r="I38" s="40" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J38" s="21">
         <v>15</v>
@@ -4904,17 +4938,17 @@
         <v>172</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="66" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q38" s="34"/>
     </row>
@@ -4935,16 +4969,16 @@
         <v>11</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G39" s="21">
         <v>21</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I39" s="40" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J39" s="21">
         <v>15</v>
@@ -4953,15 +4987,15 @@
         <v>153</v>
       </c>
       <c r="L39" s="51" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Q39" s="34"/>
     </row>
@@ -4982,13 +5016,13 @@
         <v>11</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G40" s="21">
         <v>21</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I40" s="40" t="s">
         <v>14</v>
@@ -5000,10 +5034,10 @@
         <v>166</v>
       </c>
       <c r="L40" s="37" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5092,7 +5126,7 @@
         <v>240</v>
       </c>
       <c r="L42" s="50" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>69</v>
@@ -5174,38 +5208,38 @@
         <v>44</v>
       </c>
       <c r="F44" s="43" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G44" s="44">
         <v>8</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I44" s="40" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K44" s="21">
         <v>140</v>
       </c>
       <c r="L44" s="15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="P44" s="50" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q44" s="61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:17" ht="353.25" thickBot="1" x14ac:dyDescent="0.45">
@@ -5231,41 +5265,44 @@
         <v>16</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I45" s="65" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K45" s="21">
         <v>105</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P45" s="64" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q45" s="61" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q45" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
-  <conditionalFormatting sqref="M1:M22 M24:M1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+  <conditionalFormatting sqref="M1:M22 M25:M1048576">
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M23">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M24">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -5292,16 +5329,16 @@
         <v>59</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G1" s="28">
         <v>21</v>
@@ -5310,29 +5347,29 @@
         <v>22</v>
       </c>
       <c r="I1" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="M1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="47" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="Q1" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5343,16 +5380,16 @@
         <v>59</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G2" s="28">
         <v>21</v>
@@ -5361,29 +5398,29 @@
         <v>22</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K2" s="30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" s="47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Q2" s="28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5394,45 +5431,45 @@
         <v>38</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G3" s="28">
         <v>22</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J3" s="28">
         <v>25</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="47" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5443,45 +5480,45 @@
         <v>38</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G4" s="28">
         <v>22</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J4" s="28">
         <v>25</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="47" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="Q4" s="32" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -5495,7 +5532,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5519,13 +5556,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="60" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F1" s="60" t="s">
         <v>36</v>
@@ -5700,7 +5737,7 @@
         <v>71</v>
       </c>
       <c r="M4" s="54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
@@ -5751,7 +5788,7 @@
         <v>75</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -5798,7 +5835,7 @@
         <v>77</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -5830,30 +5867,30 @@
         <v>16</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I7" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K7" s="15">
         <v>105</v>
       </c>
       <c r="L7" s="56" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P7" s="63" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q7" s="59" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -5895,10 +5932,10 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="54" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="P8" s="18" t="s">
         <v>93</v>
@@ -5946,7 +5983,7 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="14" t="s">
@@ -5994,14 +6031,16 @@
         <v>102</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>103</v>
+        <v>255</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>104</v>
+        <v>256</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="18"/>
-      <c r="Q10" s="19"/>
+      <c r="Q10" s="19" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
@@ -6020,7 +6059,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G11" s="15">
         <v>34</v>
@@ -6029,7 +6068,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>43</v>
+        <v>261</v>
       </c>
       <c r="J11" s="15" t="s">
         <v>101</v>
@@ -6038,18 +6077,16 @@
         <v>150</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>259</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="M11" s="2"/>
       <c r="N11" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6069,13 +6106,13 @@
         <v>21</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G12" s="15">
         <v>34</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>43</v>
@@ -6087,21 +6124,21 @@
         <v>180</v>
       </c>
       <c r="L12" s="56" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="59" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="243" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12">
         <v>3</v>
       </c>
@@ -6118,16 +6155,16 @@
         <v>21</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G13" s="15">
         <v>34</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J13" s="15" t="s">
         <v>101</v>
@@ -6135,17 +6172,19 @@
       <c r="K13" s="19">
         <v>60</v>
       </c>
-      <c r="L13" s="22" t="s">
-        <v>112</v>
+      <c r="L13" s="70" t="s">
+        <v>258</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>113</v>
+        <v>260</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="18"/>
+      <c r="P13" s="71" t="s">
+        <v>110</v>
+      </c>
       <c r="Q13" s="19" t="s">
-        <v>114</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6165,16 +6204,16 @@
         <v>11</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G14" s="28">
         <v>16</v>
       </c>
       <c r="H14" s="28" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J14" s="28">
         <v>14</v>
@@ -6183,16 +6222,16 @@
         <v>85</v>
       </c>
       <c r="L14" s="47" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="53"/>
       <c r="Q14" s="28" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6212,7 +6251,7 @@
         <v>21</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G15" s="15">
         <v>8</v>
@@ -6221,29 +6260,29 @@
         <v>27</v>
       </c>
       <c r="I15" s="58" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K15" s="15">
         <v>140</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="P15" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6263,38 +6302,38 @@
         <v>11</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G16" s="15">
         <v>8</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I16" s="58" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K16" s="15">
         <v>140</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P16" s="52" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q16" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6314,16 +6353,16 @@
         <v>11</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G17" s="15">
         <v>8</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I17" s="58" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>28</v>
@@ -6332,20 +6371,20 @@
         <v>140</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q17" s="59" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6365,7 +6404,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G18" s="15">
         <v>17</v>
@@ -6374,7 +6413,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J18" s="15" t="s">
         <v>28</v>
@@ -6383,18 +6422,18 @@
         <v>120</v>
       </c>
       <c r="L18" s="17" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6414,7 +6453,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G19" s="15">
         <v>16</v>
@@ -6426,26 +6465,26 @@
         <v>43</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K19" s="15">
         <v>85</v>
       </c>
       <c r="L19" s="49" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="Q19" s="19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6471,30 +6510,30 @@
         <v>16</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I20" s="45" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K20" s="15">
         <v>105</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P20" s="62" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q20" s="19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6514,36 +6553,36 @@
         <v>11</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G21" s="15">
         <v>12</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K21" s="15">
         <v>100</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="P21" s="43" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q21" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6563,36 +6602,36 @@
         <v>11</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G22" s="36">
         <v>12</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I22" s="46" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K22" s="36">
         <v>360</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="P22" s="37" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q22" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6612,36 +6651,36 @@
         <v>11</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G23" s="21">
         <v>12</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K23" s="21">
         <v>100</v>
       </c>
       <c r="L23" s="37" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="P23" s="38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q23" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6661,36 +6700,36 @@
         <v>11</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G24" s="21">
         <v>12</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K24" s="21">
         <v>360</v>
       </c>
       <c r="L24" s="37" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="P24" s="38" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="Q24" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.45">
@@ -6710,35 +6749,35 @@
         <v>21</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G25" s="34">
         <v>40</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I25" s="39" t="s">
         <v>14</v>
       </c>
       <c r="J25" s="34" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K25" s="34">
         <v>90</v>
       </c>
       <c r="L25" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="41" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="Q25" s="34"/>
     </row>
@@ -6763,10 +6802,10 @@
         <v>19</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J26" s="21">
         <v>15</v>
@@ -6775,20 +6814,20 @@
         <v>225</v>
       </c>
       <c r="L26" s="37" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="50" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="Q26" s="21" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="1:17" ht="58.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -6808,7 +6847,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G27" s="21">
         <v>19</v>
@@ -6817,7 +6856,7 @@
         <v>12</v>
       </c>
       <c r="I27" s="40" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J27" s="21">
         <v>15</v>
@@ -6826,17 +6865,17 @@
         <v>172</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="66" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="Q27" s="34"/>
     </row>
@@ -6857,16 +6896,16 @@
         <v>11</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G28" s="21">
         <v>21</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I28" s="40" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J28" s="21">
         <v>15</v>
@@ -6875,15 +6914,15 @@
         <v>153</v>
       </c>
       <c r="L28" s="51" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="Q28" s="34"/>
     </row>
@@ -6904,13 +6943,13 @@
         <v>11</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G29" s="21">
         <v>21</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="I29" s="40" t="s">
         <v>14</v>
@@ -6922,10 +6961,10 @@
         <v>166</v>
       </c>
       <c r="L29" s="37" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -6935,16 +6974,16 @@
   </sheetData>
   <autoFilter ref="A1:Q29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="M1 M30:M1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M17 M19:M29">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:N1 M30:N1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6978,13 +7017,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>36</v>
@@ -7061,7 +7100,7 @@
         <v>82</v>
       </c>
       <c r="M2" s="54" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -7152,7 +7191,7 @@
         <v>240</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>68</v>
@@ -7204,7 +7243,7 @@
         <v>79</v>
       </c>
       <c r="M5" s="54" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
@@ -7255,7 +7294,7 @@
         <v>83</v>
       </c>
       <c r="M6" s="54" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -7281,38 +7320,38 @@
         <v>44</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G7" s="44">
         <v>8</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K7" s="21">
         <v>140</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="P7" s="50" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="Q7" s="61" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -7338,37 +7377,37 @@
         <v>16</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I8" s="65" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K8" s="21">
         <v>105</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="P8" s="64" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="Q8" s="61" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M8">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7396,13 +7435,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>36</v>
@@ -7479,7 +7518,7 @@
         <v>88</v>
       </c>
       <c r="M2" s="54" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -7526,7 +7565,7 @@
         <v>89</v>
       </c>
       <c r="M3" s="54" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -7617,7 +7656,7 @@
         <v>240</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>69</v>
@@ -7684,7 +7723,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M6">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaned up some functions
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="543" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E668372-9DE6-4B03-BFF0-2FC1D4AC06FE}"/>
+  <xr:revisionPtr revIDLastSave="583" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F985A0C0-E97E-435B-8481-090209D778B1}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-15420" windowWidth="25005" windowHeight="13365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="262">
   <si>
     <t>CognitiveFunction</t>
   </si>
@@ -1780,18 +1780,6 @@
     <t>comment sensitivitý</t>
   </si>
   <si>
-    <t>1: RT 0b-2b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: difference with lag1, substract from each lag, then averages. </t>
-  </si>
-  <si>
-    <t>y, could do 1</t>
-  </si>
-  <si>
-    <t>Improve possible</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -2068,7 +2056,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -2406,7 +2394,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2561,7 +2549,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2647,7 +2635,37 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3270,8 +3288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,7 +3314,7 @@
     <col min="21" max="21" width="18.28515625" style="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -3355,9 +3373,7 @@
         <v>239</v>
       </c>
       <c r="T1" s="54"/>
-      <c r="U1" s="73" t="s">
-        <v>243</v>
-      </c>
+      <c r="U1" s="73"/>
     </row>
     <row r="2" spans="1:22" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
@@ -3372,8 +3388,8 @@
       <c r="D2" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>11</v>
+      <c r="E2" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>48</v>
@@ -3394,18 +3410,18 @@
         <v>180</v>
       </c>
       <c r="L2" s="53" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="65" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="R2" s="19">
         <v>1</v>
@@ -3414,9 +3430,7 @@
         <v>231</v>
       </c>
       <c r="T2" s="76"/>
-      <c r="U2" s="76" t="s">
-        <v>242</v>
-      </c>
+      <c r="U2" s="76"/>
     </row>
     <row r="3" spans="1:22" ht="276" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="12">
@@ -3431,8 +3445,8 @@
       <c r="D3" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>11</v>
+      <c r="E3" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>51</v>
@@ -3456,7 +3470,7 @@
         <v>54</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -3488,8 +3502,8 @@
       <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>11</v>
+      <c r="E4" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>39</v>
@@ -3520,7 +3534,7 @@
         <v>61</v>
       </c>
       <c r="P4" s="69" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="Q4" s="56" t="s">
         <v>62</v>
@@ -3547,8 +3561,8 @@
       <c r="D5" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="64" t="s">
-        <v>11</v>
+      <c r="E5" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>39</v>
@@ -3602,8 +3616,8 @@
       <c r="D6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="64" t="s">
-        <v>11</v>
+      <c r="E6" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>39</v>
@@ -3709,7 +3723,7 @@
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -3732,18 +3746,18 @@
         <v>180</v>
       </c>
       <c r="L8" s="53" t="s">
+        <v>246</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="65" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="R8" s="19">
         <v>1</v>
@@ -3751,12 +3765,8 @@
       <c r="S8" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="T8" s="76" t="s">
-        <v>240</v>
-      </c>
-      <c r="U8" s="76" t="s">
-        <v>242</v>
-      </c>
+      <c r="T8" s="76"/>
+      <c r="U8" s="76"/>
     </row>
     <row r="9" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12">
@@ -3768,7 +3778,7 @@
       <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="28" t="s">
@@ -3796,7 +3806,7 @@
         <v>209</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -3825,7 +3835,7 @@
       <c r="C10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="28" t="s">
@@ -3887,8 +3897,8 @@
       <c r="D11" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>11</v>
+      <c r="E11" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>41</v>
@@ -4109,8 +4119,8 @@
       <c r="D15" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>11</v>
+      <c r="E15" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>78</v>
@@ -4167,8 +4177,8 @@
       <c r="D16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>11</v>
+      <c r="E16" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>83</v>
@@ -4249,21 +4259,21 @@
         <v>90</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="19" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="R17" s="19">
         <v>1</v>
       </c>
       <c r="S17" s="75" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="T17" s="76"/>
       <c r="U17" s="76"/>
@@ -4307,12 +4317,12 @@
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="19" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="R18" s="19">
         <v>1</v>
@@ -4361,15 +4371,15 @@
         <v>225</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="56" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="R19" s="19">
         <v>1</v>
@@ -4377,12 +4387,8 @@
       <c r="S19" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="T19" s="76" t="s">
-        <v>241</v>
-      </c>
-      <c r="U19" s="76">
-        <v>1</v>
-      </c>
+      <c r="T19" s="76"/>
+      <c r="U19" s="76"/>
     </row>
     <row r="20" spans="1:21" ht="108" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="12">
@@ -4454,8 +4460,8 @@
       <c r="D21" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="64" t="s">
-        <v>11</v>
+      <c r="E21" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F21" s="27" t="s">
         <v>123</v>
@@ -4568,8 +4574,8 @@
       <c r="D23" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="64" t="s">
-        <v>11</v>
+      <c r="E23" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>128</v>
@@ -4627,8 +4633,8 @@
       <c r="D24" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="64" t="s">
-        <v>11</v>
+      <c r="E24" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>128</v>
@@ -4686,8 +4692,8 @@
       <c r="D25" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="64" t="s">
-        <v>11</v>
+      <c r="E25" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>148</v>
@@ -4743,8 +4749,8 @@
       <c r="D26" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="64" t="s">
-        <v>11</v>
+      <c r="E26" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>151</v>
@@ -4802,8 +4808,8 @@
       <c r="D27" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>11</v>
+      <c r="E27" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>41</v>
@@ -4859,8 +4865,8 @@
       <c r="D28" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="64" t="s">
-        <v>11</v>
+      <c r="E28" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>171</v>
@@ -4892,7 +4898,7 @@
         <v>175</v>
       </c>
       <c r="Q28" s="71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R28" s="19">
         <v>2</v>
@@ -4916,8 +4922,8 @@
       <c r="D29" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="64" t="s">
-        <v>11</v>
+      <c r="E29" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F29" s="35" t="s">
         <v>171</v>
@@ -4949,7 +4955,7 @@
         <v>175</v>
       </c>
       <c r="Q29" s="71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R29" s="19">
         <v>2</v>
@@ -4973,8 +4979,8 @@
       <c r="D30" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="64" t="s">
-        <v>11</v>
+      <c r="E30" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F30" s="38" t="s">
         <v>171</v>
@@ -5006,7 +5012,7 @@
         <v>175</v>
       </c>
       <c r="Q30" s="71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R30" s="19">
         <v>2</v>
@@ -5030,8 +5036,8 @@
       <c r="D31" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E31" s="64" t="s">
-        <v>11</v>
+      <c r="E31" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F31" s="38" t="s">
         <v>171</v>
@@ -5063,7 +5069,7 @@
         <v>175</v>
       </c>
       <c r="Q31" s="71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R31" s="19">
         <v>2</v>
@@ -5087,7 +5093,7 @@
       <c r="D32" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="38" t="s">
@@ -5113,7 +5119,7 @@
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>210</v>
@@ -5146,8 +5152,8 @@
       <c r="D33" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="64" t="s">
-        <v>11</v>
+      <c r="E33" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F33" s="41"/>
       <c r="G33" s="21">
@@ -5201,8 +5207,8 @@
       <c r="D34" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="64" t="s">
-        <v>11</v>
+      <c r="E34" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F34" s="38" t="s">
         <v>191</v>
@@ -5256,8 +5262,8 @@
       <c r="D35" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="64" t="s">
-        <v>11</v>
+      <c r="E35" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F35" s="38" t="s">
         <v>191</v>
@@ -5311,8 +5317,8 @@
       <c r="D36" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="64" t="s">
-        <v>11</v>
+      <c r="E36" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F36" s="38" t="s">
         <v>200</v>
@@ -5384,18 +5390,18 @@
         <v>180</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="65" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q37" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="R37" s="19">
         <v>1</v>
@@ -5403,14 +5409,10 @@
       <c r="S37" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="T37" s="76" t="s">
-        <v>240</v>
-      </c>
-      <c r="U37" s="76" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="T37" s="76"/>
+      <c r="U37" s="76"/>
+    </row>
+    <row r="38" spans="1:21" ht="276" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="33">
         <v>1</v>
       </c>
@@ -5420,7 +5422,7 @@
       <c r="C38" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E38" s="21" t="s">
@@ -5452,7 +5454,7 @@
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="38" t="s">
+      <c r="P38" s="78" t="s">
         <v>55</v>
       </c>
       <c r="Q38" s="21" t="s">
@@ -5477,7 +5479,7 @@
       <c r="C39" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E39" s="21" t="s">
@@ -5536,7 +5538,7 @@
       <c r="C40" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E40" s="28" t="s">
@@ -5595,7 +5597,7 @@
       <c r="C41" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E41" s="28" t="s">
@@ -5647,46 +5649,46 @@
   </sheetData>
   <autoFilter ref="A1:U41" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
   <conditionalFormatting sqref="M19">
-    <cfRule type="duplicateValues" dxfId="32" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20">
-    <cfRule type="duplicateValues" dxfId="31" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M21:M1048576 M1:M18">
-    <cfRule type="duplicateValues" dxfId="30" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
-    <cfRule type="duplicateValues" dxfId="29" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5">
-    <cfRule type="duplicateValues" dxfId="28" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="duplicateValues" dxfId="27" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7">
-    <cfRule type="duplicateValues" dxfId="26" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="duplicateValues" dxfId="24" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N39">
-    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O25">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O32">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5696,7 +5698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C34885-F57D-4289-A4BD-D56F75A94A93}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -5910,10 +5912,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="57" zoomScaleNormal="29" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="L1" zoomScale="59" zoomScaleNormal="29" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5936,7 +5938,7 @@
     <col min="20" max="21" width="9.140625" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
@@ -5995,9 +5997,7 @@
         <v>239</v>
       </c>
       <c r="T1" s="54"/>
-      <c r="U1" s="73" t="s">
-        <v>243</v>
-      </c>
+      <c r="U1" s="73"/>
     </row>
     <row r="2" spans="1:22" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
@@ -6034,18 +6034,18 @@
         <v>180</v>
       </c>
       <c r="L2" s="53" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="65" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="R2" s="19">
         <v>1</v>
@@ -6054,9 +6054,7 @@
         <v>231</v>
       </c>
       <c r="T2" s="76"/>
-      <c r="U2" s="76" t="s">
-        <v>242</v>
-      </c>
+      <c r="U2" s="76"/>
     </row>
     <row r="3" spans="1:22" ht="276" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="12">
@@ -6071,8 +6069,8 @@
       <c r="D3" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>11</v>
+      <c r="E3" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>51</v>
@@ -6096,7 +6094,7 @@
         <v>54</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -6128,8 +6126,8 @@
       <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>11</v>
+      <c r="E4" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>39</v>
@@ -6160,7 +6158,7 @@
         <v>61</v>
       </c>
       <c r="P4" s="69" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="Q4" s="56" t="s">
         <v>62</v>
@@ -6187,8 +6185,8 @@
       <c r="D5" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="64" t="s">
-        <v>11</v>
+      <c r="E5" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>39</v>
@@ -6242,8 +6240,8 @@
       <c r="D6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="64" t="s">
-        <v>11</v>
+      <c r="E6" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>39</v>
@@ -6297,8 +6295,8 @@
       <c r="D7" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>11</v>
+      <c r="E7" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>41</v>
@@ -6354,8 +6352,8 @@
       <c r="D8" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>11</v>
+      <c r="E8" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>78</v>
@@ -6412,8 +6410,8 @@
       <c r="D9" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>11</v>
+      <c r="E9" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>83</v>
@@ -6456,111 +6454,113 @@
       <c r="T9" s="76"/>
       <c r="U9" s="76"/>
     </row>
-    <row r="10" spans="1:22" ht="45.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="25">
-        <v>3</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="15">
-        <v>34</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K10" s="15">
-        <v>180</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>90</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="28">
+        <v>16</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="28">
+        <v>14</v>
+      </c>
+      <c r="K10" s="28">
+        <v>85</v>
+      </c>
+      <c r="L10" s="68" t="s">
+        <v>126</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>256</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="19" t="s">
-        <v>258</v>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="67" t="s">
+        <v>234</v>
       </c>
       <c r="R10" s="19">
         <v>1</v>
       </c>
       <c r="S10" s="75" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="T10" s="76"/>
       <c r="U10" s="76"/>
     </row>
     <row r="11" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
-        <v>3</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="G11" s="15">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>43</v>
+        <v>136</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>220</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="K11" s="15">
-        <v>150</v>
-      </c>
-      <c r="L11" s="53" t="s">
-        <v>92</v>
+        <v>140</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>138</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="18"/>
+        <v>139</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P11" s="50" t="s">
+        <v>134</v>
+      </c>
       <c r="Q11" s="19" t="s">
-        <v>260</v>
+        <v>135</v>
       </c>
       <c r="R11" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11" s="75" t="s">
         <v>231</v>
@@ -6568,117 +6568,115 @@
       <c r="T11" s="76"/>
       <c r="U11" s="76"/>
     </row>
-    <row r="12" spans="1:22" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="D12" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="G12" s="15">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>43</v>
+        <v>136</v>
+      </c>
+      <c r="I12" s="55" t="s">
+        <v>221</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K12" s="19">
-        <v>180</v>
-      </c>
-      <c r="L12" s="53" t="s">
-        <v>225</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>264</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="K12" s="15">
+        <v>140</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="18"/>
+        <v>142</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P12" s="18" t="s">
+        <v>134</v>
+      </c>
       <c r="Q12" s="56" t="s">
-        <v>265</v>
+        <v>135</v>
       </c>
       <c r="R12" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="T12" s="76" t="s">
-        <v>241</v>
-      </c>
-      <c r="U12" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="123" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="T12" s="76"/>
+      <c r="U12" s="76"/>
+    </row>
+    <row r="13" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12">
+        <v>7</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="G13" s="15">
+        <v>17</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="15">
+        <v>120</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="56" t="s">
+        <v>232</v>
+      </c>
+      <c r="R13" s="19">
         <v>3</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" s="15">
-        <v>34</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="K13" s="19">
-        <v>60</v>
-      </c>
-      <c r="L13" s="65" t="s">
-        <v>226</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="66" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q13" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="R13" s="19">
-        <v>2</v>
       </c>
       <c r="S13" s="75" t="s">
         <v>231</v>
@@ -6686,54 +6684,58 @@
       <c r="T13" s="76"/>
       <c r="U13" s="76"/>
     </row>
-    <row r="14" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="25">
-        <v>5</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>25</v>
+    <row r="14" spans="1:22" ht="108" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="12">
+        <v>8</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="D14" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="G14" s="28">
+      <c r="E14" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="15">
         <v>16</v>
       </c>
-      <c r="H14" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="67" t="s">
-        <v>125</v>
-      </c>
-      <c r="J14" s="28">
-        <v>14</v>
-      </c>
-      <c r="K14" s="28">
+      <c r="H14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="15">
         <v>85</v>
       </c>
-      <c r="L14" s="68" t="s">
-        <v>126</v>
+      <c r="L14" s="70" t="s">
+        <v>153</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N14" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="O14" s="2"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="67" t="s">
-        <v>234</v>
+      <c r="P14" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q14" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="R14" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S14" s="75" t="s">
         <v>231</v>
@@ -6741,58 +6743,56 @@
       <c r="T14" s="76"/>
       <c r="U14" s="76"/>
     </row>
-    <row r="15" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="12">
-        <v>6</v>
+    <row r="15" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="33">
+        <v>9</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="D15" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="G15" s="15">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="55" t="s">
-        <v>220</v>
+        <v>136</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>158</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="K15" s="15">
-        <v>140</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>131</v>
+        <v>105</v>
+      </c>
+      <c r="L15" s="53" t="s">
+        <v>160</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="N15" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="P15" s="18" t="s">
-        <v>134</v>
+        <v>161</v>
+      </c>
+      <c r="P15" s="58" t="s">
+        <v>162</v>
       </c>
       <c r="Q15" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="R15" s="19">
-        <v>2</v>
+        <v>163</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>236</v>
       </c>
       <c r="S15" s="75" t="s">
         <v>231</v>
@@ -6800,55 +6800,53 @@
       <c r="T15" s="76"/>
       <c r="U15" s="76"/>
     </row>
-    <row r="16" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:22" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="12">
-        <v>6</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="64" t="s">
-        <v>11</v>
+      <c r="E16" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
       <c r="G16" s="15">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I16" s="55" t="s">
-        <v>220</v>
+        <v>19</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>172</v>
       </c>
       <c r="J16" s="15" t="s">
         <v>137</v>
       </c>
       <c r="K16" s="15">
-        <v>140</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>138</v>
+        <v>100</v>
+      </c>
+      <c r="L16" s="53" t="s">
+        <v>173</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="P16" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q16" s="19" t="s">
-        <v>135</v>
+        <v>174</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q16" s="71" t="s">
+        <v>243</v>
       </c>
       <c r="R16" s="19">
         <v>2</v>
@@ -6859,55 +6857,53 @@
       <c r="T16" s="76"/>
       <c r="U16" s="76"/>
     </row>
-    <row r="17" spans="1:21" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="12">
-        <v>6</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D17" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="G17" s="15">
-        <v>8</v>
+      <c r="E17" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="36">
+        <v>12</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I17" s="55" t="s">
-        <v>221</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="15">
-        <v>140</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>141</v>
+        <v>19</v>
+      </c>
+      <c r="I17" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="K17" s="36">
+        <v>360</v>
+      </c>
+      <c r="L17" s="63" t="s">
+        <v>176</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="P17" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q17" s="56" t="s">
-        <v>135</v>
+        <v>177</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q17" s="71" t="s">
+        <v>243</v>
       </c>
       <c r="R17" s="19">
         <v>2</v>
@@ -6918,56 +6914,56 @@
       <c r="T17" s="76"/>
       <c r="U17" s="76"/>
     </row>
-    <row r="18" spans="1:21" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12">
-        <v>7</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="15">
-        <v>17</v>
+      <c r="E18" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="G18" s="21">
+        <v>12</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18" s="15">
-        <v>120</v>
-      </c>
-      <c r="L18" s="53" t="s">
-        <v>150</v>
+        <v>19</v>
+      </c>
+      <c r="I18" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" s="21">
+        <v>100</v>
+      </c>
+      <c r="L18" s="37" t="s">
+        <v>179</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="56" t="s">
-        <v>232</v>
+        <v>180</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q18" s="71" t="s">
+        <v>243</v>
       </c>
       <c r="R18" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S18" s="75" t="s">
         <v>231</v>
@@ -6975,55 +6971,53 @@
       <c r="T18" s="76"/>
       <c r="U18" s="76"/>
     </row>
-    <row r="19" spans="1:21" ht="108" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="12">
-        <v>8</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D19" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="G19" s="15">
-        <v>16</v>
+      <c r="E19" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="21">
+        <v>12</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="K19" s="15">
-        <v>85</v>
-      </c>
-      <c r="L19" s="70" t="s">
-        <v>153</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>154</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="I19" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="K19" s="21">
+        <v>360</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="O19" s="2"/>
-      <c r="P19" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q19" s="19" t="s">
-        <v>157</v>
+      <c r="P19" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q19" s="71" t="s">
+        <v>243</v>
       </c>
       <c r="R19" s="19">
         <v>2</v>
@@ -7034,56 +7028,54 @@
       <c r="T19" s="76"/>
       <c r="U19" s="76"/>
     </row>
-    <row r="20" spans="1:21" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="33">
-        <v>9</v>
-      </c>
-      <c r="B20" s="24" t="s">
+    <row r="20" spans="1:21" ht="117.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="12">
+        <v>12</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="41"/>
+      <c r="G20" s="21">
+        <v>19</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="I20" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="J20" s="21">
         <v>15</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="15">
-        <v>16</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="K20" s="15">
-        <v>105</v>
-      </c>
-      <c r="L20" s="53" t="s">
-        <v>160</v>
+      <c r="K20" s="21">
+        <v>225</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="P20" s="58" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q20" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="R20" s="19" t="s">
-        <v>236</v>
+      <c r="N20" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q20" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="R20" s="19">
+        <v>2</v>
       </c>
       <c r="S20" s="75" t="s">
         <v>231</v>
@@ -7091,56 +7083,54 @@
       <c r="T20" s="76"/>
       <c r="U20" s="76"/>
     </row>
-    <row r="21" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" ht="117.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="12">
-        <v>10</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="D21" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="G21" s="15">
+      <c r="E21" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="G21" s="21">
+        <v>19</v>
+      </c>
+      <c r="H21" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H21" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="J21" s="21">
+        <v>15</v>
+      </c>
+      <c r="K21" s="21">
         <v>172</v>
       </c>
-      <c r="J21" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="K21" s="15">
-        <v>100</v>
-      </c>
-      <c r="L21" s="53" t="s">
-        <v>173</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2" t="s">
-        <v>174</v>
-      </c>
+      <c r="L21" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="43" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q21" s="71" t="s">
-        <v>247</v>
-      </c>
+      <c r="P21" s="62" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q21" s="34"/>
       <c r="R21" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S21" s="75" t="s">
         <v>231</v>
@@ -7148,56 +7138,54 @@
       <c r="T21" s="76"/>
       <c r="U21" s="76"/>
     </row>
-    <row r="22" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" ht="231.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
-        <v>10</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="D22" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="G22" s="36">
-        <v>12</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="K22" s="36">
-        <v>360</v>
-      </c>
-      <c r="L22" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2" t="s">
-        <v>177</v>
-      </c>
+      <c r="E22" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="G22" s="21">
+        <v>21</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="J22" s="21">
+        <v>15</v>
+      </c>
+      <c r="K22" s="21">
+        <v>153</v>
+      </c>
+      <c r="L22" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="37" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q22" s="71" t="s">
-        <v>247</v>
-      </c>
+      <c r="P22" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q22" s="34"/>
       <c r="R22" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S22" s="75" t="s">
         <v>231</v>
@@ -7205,54 +7193,50 @@
       <c r="T22" s="76"/>
       <c r="U22" s="76"/>
     </row>
-    <row r="23" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12">
-        <v>10</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>35</v>
       </c>
       <c r="D23" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="64" t="s">
-        <v>11</v>
+      <c r="E23" s="63" t="s">
+        <v>17</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="G23" s="21">
-        <v>12</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>201</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>178</v>
+        <v>14</v>
+      </c>
+      <c r="J23" s="21">
+        <v>15</v>
       </c>
       <c r="K23" s="21">
-        <v>100</v>
+        <v>166</v>
       </c>
       <c r="L23" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2" t="s">
-        <v>180</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q23" s="71" t="s">
-        <v>247</v>
-      </c>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="34"/>
       <c r="R23" s="19">
         <v>2</v>
       </c>
@@ -7308,7 +7292,7 @@
         <v>175</v>
       </c>
       <c r="Q24" s="71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="R24" s="19">
         <v>2</v>
@@ -7358,7 +7342,7 @@
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>210</v>
@@ -7596,38 +7580,391 @@
       <c r="T29" s="76"/>
       <c r="U29" s="76"/>
     </row>
+    <row r="30" spans="1:21" ht="45.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="25">
+        <v>3</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="15">
+        <v>34</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K30" s="15">
+        <v>180</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="R30" s="19">
+        <v>1</v>
+      </c>
+      <c r="S30" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="T30" s="76"/>
+      <c r="U30" s="76"/>
+    </row>
+    <row r="31" spans="1:21" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="12">
+        <v>3</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="15">
+        <v>34</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="15">
+        <v>150</v>
+      </c>
+      <c r="L31" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="R31" s="19">
+        <v>1</v>
+      </c>
+      <c r="S31" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="T31" s="76"/>
+      <c r="U31" s="76"/>
+    </row>
+    <row r="32" spans="1:21" ht="174.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="12">
+        <v>3</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="15">
+        <v>34</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" s="19">
+        <v>180</v>
+      </c>
+      <c r="L32" s="53" t="s">
+        <v>225</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="R32" s="19">
+        <v>1</v>
+      </c>
+      <c r="S32" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="T32" s="76"/>
+      <c r="U32" s="76"/>
+    </row>
+    <row r="33" spans="1:21" ht="123" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="12">
+        <v>3</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="15">
+        <v>34</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K33" s="19">
+        <v>60</v>
+      </c>
+      <c r="L33" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q33" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="R33" s="19">
+        <v>2</v>
+      </c>
+      <c r="S33" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="T33" s="76"/>
+      <c r="U33" s="76"/>
+    </row>
+    <row r="34" spans="1:21" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="12">
+        <v>6</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="15">
+        <v>8</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="K34" s="15">
+        <v>140</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="P34" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q34" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="R34" s="19">
+        <v>2</v>
+      </c>
+      <c r="S34" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="T34" s="76"/>
+      <c r="U34" s="76"/>
+    </row>
+    <row r="35" spans="1:21" ht="78" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="12">
+        <v>11</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="G35" s="34">
+        <v>40</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="K35" s="34">
+        <v>90</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="P35" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q35" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="R35" s="19">
+        <v>1</v>
+      </c>
+      <c r="S35" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="T35" s="76"/>
+      <c r="U35" s="76"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M12">
-    <cfRule type="duplicateValues" dxfId="18" priority="4"/>
+  <conditionalFormatting sqref="M1:M23">
+    <cfRule type="duplicateValues" dxfId="21" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M13">
-    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+  <conditionalFormatting sqref="M24:M29">
+    <cfRule type="duplicateValues" dxfId="20" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M29 M1:M11">
-    <cfRule type="duplicateValues" dxfId="16" priority="8"/>
+  <conditionalFormatting sqref="M32">
+    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M30:M1048564">
-    <cfRule type="duplicateValues" dxfId="15" priority="24"/>
+  <conditionalFormatting sqref="M33">
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M34:M35 M30:M31">
+    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M36:M1048564">
+    <cfRule type="duplicateValues" dxfId="16" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1048565:M1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1048565:N1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
+    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N5">
     <cfRule type="duplicateValues" dxfId="12" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="N6">
     <cfRule type="duplicateValues" dxfId="11" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="O13">
     <cfRule type="duplicateValues" dxfId="10" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+  <conditionalFormatting sqref="O25">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O25">
+  <conditionalFormatting sqref="O35">
     <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7639,8 +7976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5538A5-2CE0-400F-BF9C-B504D5DC3739}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView zoomScale="69" workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:U8"/>
+    <sheetView topLeftCell="L1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7714,9 +8051,7 @@
         <v>239</v>
       </c>
       <c r="T1" s="54"/>
-      <c r="U1" s="73" t="s">
-        <v>243</v>
-      </c>
+      <c r="U1" s="73"/>
     </row>
     <row r="2" spans="1:21" ht="345.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
@@ -7783,7 +8118,7 @@
       <c r="C3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="28" t="s">
@@ -7806,18 +8141,18 @@
         <v>180</v>
       </c>
       <c r="L3" s="53" t="s">
+        <v>246</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="65" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q3" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="R3" s="19">
         <v>1</v>
@@ -7825,12 +8160,8 @@
       <c r="S3" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="T3" s="76" t="s">
-        <v>240</v>
-      </c>
-      <c r="U3" s="76" t="s">
-        <v>242</v>
-      </c>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
     </row>
     <row r="4" spans="1:21" ht="345.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12">
@@ -7842,7 +8173,7 @@
       <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E4" s="28" t="s">
@@ -7870,7 +8201,7 @@
         <v>209</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -7899,7 +8230,7 @@
       <c r="C5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="28" t="s">
@@ -8013,7 +8344,7 @@
       <c r="C7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="28" t="s">
@@ -8072,7 +8403,7 @@
       <c r="C8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="28" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -8143,7 +8474,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:U6"/>
+      <selection activeCell="T1" sqref="T1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8211,9 +8542,7 @@
         <v>239</v>
       </c>
       <c r="T1" s="54"/>
-      <c r="U1" s="73" t="s">
-        <v>243</v>
-      </c>
+      <c r="U1" s="73"/>
     </row>
     <row r="2" spans="1:21" ht="345.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
@@ -8358,18 +8687,18 @@
         <v>180</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="65" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="R4" s="19">
         <v>1</v>
@@ -8377,12 +8706,8 @@
       <c r="S4" s="75" t="s">
         <v>231</v>
       </c>
-      <c r="T4" s="76" t="s">
-        <v>240</v>
-      </c>
-      <c r="U4" s="76" t="s">
-        <v>242</v>
-      </c>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
     </row>
     <row r="5" spans="1:21" ht="345.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="33">
@@ -8394,7 +8719,7 @@
       <c r="C5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="21" t="s">
@@ -8451,7 +8776,7 @@
       <c r="C6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="21" t="s">

</xml_diff>

<commit_message>
Devided ACC and RT markdown files. Included Id 13 in dataset + EF sheet with ID 13
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="584" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0800A3AB-032C-471E-93B6-011876A7691E}"/>
+  <xr:revisionPtr revIDLastSave="617" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF530F7E-DA80-4F11-A046-A5F1EE82C1CA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="-15015" windowWidth="21600" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Low Dose'!$A$1:$Q$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$U$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$U$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="268">
   <si>
     <t>CognitiveFunction</t>
   </si>
@@ -2052,6 +2052,24 @@
   </si>
   <si>
     <t>EF_sensitivity</t>
+  </si>
+  <si>
+    <t>Vollenweider et al. (1998)</t>
+  </si>
+  <si>
+    <t>delayed response task (DRT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 2:
+Ketanserin
+RT (Pla + Pla)  0.71 (±0.07)- RT Pla + Psi  1.10 (±0.12)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">increased RT </t>
+  </si>
+  <si>
+    <t>Took ketanserin gorup</t>
   </si>
 </sst>
 </file>
@@ -2399,7 +2417,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2632,6 +2650,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3289,10 +3310,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,7 +3328,7 @@
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" customWidth="1"/>
     <col min="14" max="14" width="17.5703125" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="16" max="16" width="20.28515625" customWidth="1"/>
@@ -3430,7 +3452,7 @@
         <v>1</v>
       </c>
       <c r="S2" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T2" s="76"/>
       <c r="U2" s="76"/>
@@ -3487,7 +3509,7 @@
         <v>3</v>
       </c>
       <c r="S3" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T3" s="76"/>
       <c r="U3" s="76"/>
@@ -3546,7 +3568,7 @@
         <v>3</v>
       </c>
       <c r="S4" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T4" s="76"/>
       <c r="U4" s="76"/>
@@ -3601,7 +3623,7 @@
         <v>3</v>
       </c>
       <c r="S5" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T5" s="76"/>
       <c r="U5" s="76"/>
@@ -3656,7 +3678,7 @@
         <v>3</v>
       </c>
       <c r="S6" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T6" s="76"/>
       <c r="U6" s="76"/>
@@ -3711,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="S7" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T7" s="76"/>
       <c r="U7" s="76"/>
@@ -3766,7 +3788,7 @@
         <v>1</v>
       </c>
       <c r="S8" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T8" s="76"/>
       <c r="U8" s="76"/>
@@ -3823,7 +3845,7 @@
         <v>3</v>
       </c>
       <c r="S9" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T9" s="76"/>
       <c r="U9" s="76"/>
@@ -3882,7 +3904,7 @@
         <v>3</v>
       </c>
       <c r="S10" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T10" s="76"/>
       <c r="U10" s="76"/>
@@ -3939,7 +3961,7 @@
         <v>236</v>
       </c>
       <c r="S11" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T11" s="76"/>
       <c r="U11" s="76"/>
@@ -3994,7 +4016,7 @@
         <v>3</v>
       </c>
       <c r="S12" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T12" s="76"/>
       <c r="U12" s="76"/>
@@ -4049,7 +4071,7 @@
         <v>3</v>
       </c>
       <c r="S13" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T13" s="76"/>
       <c r="U13" s="76"/>
@@ -4104,7 +4126,7 @@
         <v>3</v>
       </c>
       <c r="S14" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T14" s="76"/>
       <c r="U14" s="76"/>
@@ -4161,7 +4183,7 @@
         <v>2</v>
       </c>
       <c r="S15" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T15" s="76"/>
       <c r="U15" s="76"/>
@@ -4219,7 +4241,7 @@
         <v>1</v>
       </c>
       <c r="S16" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T16" s="76"/>
       <c r="U16" s="76"/>
@@ -4331,7 +4353,7 @@
         <v>1</v>
       </c>
       <c r="S18" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T18" s="76"/>
       <c r="U18" s="76"/>
@@ -4388,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="S19" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T19" s="76"/>
       <c r="U19" s="76"/>
@@ -4421,8 +4443,8 @@
       <c r="I20" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="15" t="s">
-        <v>89</v>
+      <c r="J20" s="15">
+        <v>0.79500000000000004</v>
       </c>
       <c r="K20" s="19">
         <v>60</v>
@@ -4445,7 +4467,7 @@
         <v>2</v>
       </c>
       <c r="S20" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T20" s="76"/>
       <c r="U20" s="76"/>
@@ -4500,7 +4522,7 @@
         <v>1</v>
       </c>
       <c r="S21" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T21" s="76"/>
       <c r="U21" s="76"/>
@@ -4559,7 +4581,7 @@
         <v>2</v>
       </c>
       <c r="S22" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T22" s="76"/>
       <c r="U22" s="76"/>
@@ -4618,7 +4640,7 @@
         <v>2</v>
       </c>
       <c r="S23" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T23" s="76"/>
       <c r="U23" s="76"/>
@@ -4677,7 +4699,7 @@
         <v>2</v>
       </c>
       <c r="S24" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T24" s="76"/>
       <c r="U24" s="76"/>
@@ -4734,7 +4756,7 @@
         <v>3</v>
       </c>
       <c r="S25" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T25" s="76"/>
       <c r="U25" s="76"/>
@@ -4793,7 +4815,7 @@
         <v>2</v>
       </c>
       <c r="S26" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T26" s="76"/>
       <c r="U26" s="76"/>
@@ -4850,7 +4872,7 @@
         <v>236</v>
       </c>
       <c r="S27" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T27" s="76"/>
       <c r="U27" s="76"/>
@@ -4907,7 +4929,7 @@
         <v>2</v>
       </c>
       <c r="S28" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T28" s="76"/>
       <c r="U28" s="76"/>
@@ -4964,7 +4986,7 @@
         <v>2</v>
       </c>
       <c r="S29" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T29" s="76"/>
       <c r="U29" s="76"/>
@@ -5021,7 +5043,7 @@
         <v>2</v>
       </c>
       <c r="S30" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T30" s="76"/>
       <c r="U30" s="76"/>
@@ -5078,7 +5100,7 @@
         <v>2</v>
       </c>
       <c r="S31" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T31" s="76"/>
       <c r="U31" s="76"/>
@@ -5137,7 +5159,7 @@
         <v>1</v>
       </c>
       <c r="S32" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T32" s="76"/>
       <c r="U32" s="76"/>
@@ -5192,7 +5214,7 @@
         <v>2</v>
       </c>
       <c r="S33" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T33" s="76"/>
       <c r="U33" s="76"/>
@@ -5247,7 +5269,7 @@
         <v>3</v>
       </c>
       <c r="S34" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T34" s="76"/>
       <c r="U34" s="76"/>
@@ -5302,7 +5324,7 @@
         <v>3</v>
       </c>
       <c r="S35" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T35" s="76"/>
       <c r="U35" s="76"/>
@@ -5355,7 +5377,7 @@
         <v>2</v>
       </c>
       <c r="S36" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T36" s="76"/>
       <c r="U36" s="76"/>
@@ -5410,7 +5432,7 @@
         <v>1</v>
       </c>
       <c r="S37" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T37" s="76"/>
       <c r="U37" s="76"/>
@@ -5467,7 +5489,7 @@
         <v>3</v>
       </c>
       <c r="S38" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T38" s="76"/>
       <c r="U38" s="76"/>
@@ -5526,7 +5548,7 @@
         <v>3</v>
       </c>
       <c r="S39" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T39" s="76"/>
       <c r="U39" s="76"/>
@@ -5585,7 +5607,7 @@
         <v>2</v>
       </c>
       <c r="S40" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T40" s="76"/>
       <c r="U40" s="76"/>
@@ -5644,20 +5666,71 @@
         <v>2</v>
       </c>
       <c r="S41" s="75" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="T41" s="76"/>
       <c r="U41" s="76"/>
     </row>
+    <row r="42" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="79">
+        <v>13</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="G42" s="21">
+        <v>25</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21">
+        <v>17.5</v>
+      </c>
+      <c r="K42" s="21">
+        <v>80</v>
+      </c>
+      <c r="L42" s="71" t="s">
+        <v>265</v>
+      </c>
+      <c r="M42" s="21">
+        <v>1.78</v>
+      </c>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="R42" s="21"/>
+      <c r="S42" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="T42" s="21"/>
+      <c r="U42" s="21"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:U41" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
+  <autoFilter ref="A1:U42" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
   <conditionalFormatting sqref="M19">
     <cfRule type="duplicateValues" dxfId="35" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M20">
     <cfRule type="duplicateValues" dxfId="34" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M21:M1048576 M1:M18">
+  <conditionalFormatting sqref="M21:M41 M1:M18 M43:M1048576">
     <cfRule type="duplicateValues" dxfId="33" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4">
@@ -5694,6 +5767,7 @@
     <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
udpate id 13 ES
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="617" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF530F7E-DA80-4F11-A046-A5F1EE82C1CA}"/>
+  <xr:revisionPtr revIDLastSave="621" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEFDCAF8-C9B6-4E10-AB80-A61AFDB54A17}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="-15015" windowWidth="21600" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2060,16 +2060,22 @@
     <t>delayed response task (DRT)</t>
   </si>
   <si>
-    <t xml:space="preserve">Figure 2:
-Ketanserin
-RT (Pla + Pla)  0.71 (±0.07)- RT Pla + Psi  1.10 (±0.12)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">increased RT </t>
   </si>
   <si>
-    <t>Took ketanserin gorup</t>
+    <t>Figure 2:  mean(+/- se)
+Ketanserin:
+Pla-pla: 0.71 (0.06)
+Pla-psil: 1.08 (0.14)
+Risperidone:
+Pla-pla: 0.79 (0.07)
+Pla-psil: 1.15 (0.07)
+Haloperidol:
+Pla-pla: 0.75 (0.04)
+Pla-psil: 1.23 (0.17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Took cohens d across 3 groups. </t>
   </si>
 </sst>
 </file>
@@ -2651,7 +2657,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3313,8 +3319,8 @@
   <dimension ref="A1:V42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5671,7 +5677,7 @@
       <c r="T41" s="76"/>
       <c r="U41" s="76"/>
     </row>
-    <row r="42" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:21" ht="186.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="79">
         <v>13</v>
       </c>
@@ -5688,7 +5694,7 @@
         <v>17</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G42" s="21">
         <v>25</v>
@@ -5704,10 +5710,10 @@
         <v>80</v>
       </c>
       <c r="L42" s="71" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M42" s="21">
-        <v>1.78</v>
+        <v>1.75</v>
       </c>
       <c r="N42" s="21"/>
       <c r="O42" s="21"/>

</xml_diff>

<commit_message>
updated name of column Timepoint (min) to Timepoint in Overview_Studies.xlsx
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/Meta analysis Literature final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="627" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BD43E6B-2684-4DD7-824B-0A403F71A762}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B272F0-9865-4FE5-8ECE-D5905CF8D327}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Low Dose'!$A$1:$Q$29</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$U$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$V$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="270">
   <si>
     <t>CognitiveFunction</t>
   </si>
@@ -2076,6 +2076,12 @@
   </si>
   <si>
     <t xml:space="preserve">Took cohens d across 3 groups. </t>
+  </si>
+  <si>
+    <t>ES_ID</t>
+  </si>
+  <si>
+    <t>Timepoint</t>
   </si>
 </sst>
 </file>
@@ -2423,7 +2429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2658,6 +2664,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3316,2460 +3328,2504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I42" sqref="I42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" customWidth="1"/>
-    <col min="17" max="17" width="32.42578125" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="28" style="74" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="74"/>
-    <col min="21" max="21" width="18.28515625" style="74" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28" style="74" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="74"/>
+    <col min="22" max="22" width="18.28515625" style="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="80" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="S1" s="72" t="s">
+      <c r="T1" s="72" t="s">
         <v>239</v>
       </c>
-      <c r="T1" s="54"/>
-      <c r="U1" s="73"/>
-    </row>
-    <row r="2" spans="1:22" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="U1" s="54"/>
+      <c r="V1" s="73"/>
+    </row>
+    <row r="2" spans="1:23" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="15">
+      <c r="H2" s="15">
         <v>19</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="J2" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="15">
+      <c r="K2" s="15">
         <v>10</v>
       </c>
-      <c r="K2" s="15">
+      <c r="L2" s="15">
         <v>180</v>
       </c>
-      <c r="L2" s="53" t="s">
+      <c r="M2" s="53" t="s">
         <v>244</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="65" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="R2" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="R2" s="19">
+      <c r="S2" s="19">
         <v>1</v>
       </c>
-      <c r="S2" s="75" t="s">
+      <c r="T2" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T2" s="76"/>
       <c r="U2" s="76"/>
-    </row>
-    <row r="3" spans="1:22" ht="276" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V2" s="76"/>
+    </row>
+    <row r="3" spans="1:23" ht="276" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="79"/>
+      <c r="C3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="15">
+      <c r="H3" s="15">
         <v>20</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="15">
+      <c r="L3" s="15">
         <v>240</v>
       </c>
-      <c r="L3" s="47" t="s">
+      <c r="M3" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="69" t="s">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="R3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R3" s="19">
+      <c r="S3" s="19">
         <v>3</v>
       </c>
-      <c r="S3" s="75" t="s">
+      <c r="T3" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T3" s="76"/>
       <c r="U3" s="76"/>
-    </row>
-    <row r="4" spans="1:22" ht="321.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V3" s="76"/>
+    </row>
+    <row r="4" spans="1:23" ht="321.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="D4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="15">
+      <c r="H4" s="15">
         <v>14</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="J4" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="15">
         <v>10</v>
       </c>
-      <c r="K4" s="15">
+      <c r="L4" s="15">
         <v>120</v>
       </c>
-      <c r="L4" s="53" t="s">
+      <c r="M4" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52" t="s">
+      <c r="N4" s="52"/>
+      <c r="O4" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="69" t="s">
+      <c r="Q4" s="69" t="s">
         <v>240</v>
       </c>
-      <c r="Q4" s="56" t="s">
+      <c r="R4" s="56" t="s">
         <v>62</v>
       </c>
-      <c r="R4" s="19">
+      <c r="S4" s="19">
         <v>3</v>
       </c>
-      <c r="S4" s="75" t="s">
+      <c r="T4" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T4" s="76"/>
       <c r="U4" s="76"/>
-    </row>
-    <row r="5" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V4" s="76"/>
+    </row>
+    <row r="5" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="79"/>
+      <c r="C5" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="15">
+      <c r="H5" s="15">
         <v>14</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="J5" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="15">
+      <c r="K5" s="15">
         <v>10</v>
       </c>
-      <c r="K5" s="15">
+      <c r="L5" s="15">
         <v>240</v>
       </c>
-      <c r="L5" s="77" t="s">
+      <c r="M5" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52" t="s">
+      <c r="N5" s="52"/>
+      <c r="O5" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="57" t="s">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="R5" s="19">
+      <c r="S5" s="19">
         <v>3</v>
       </c>
-      <c r="S5" s="75" t="s">
+      <c r="T5" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T5" s="76"/>
       <c r="U5" s="76"/>
-    </row>
-    <row r="6" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V5" s="76"/>
+    </row>
+    <row r="6" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="12">
         <v>1</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="79"/>
+      <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="15">
+      <c r="H6" s="15">
         <v>14</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="J6" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="15">
+      <c r="K6" s="15">
         <v>10</v>
       </c>
-      <c r="K6" s="15">
+      <c r="L6" s="15">
         <v>360</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="M6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="52"/>
+      <c r="O6" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="34" t="s">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="19">
+      <c r="S6" s="19">
         <v>3</v>
       </c>
-      <c r="S6" s="75" t="s">
+      <c r="T6" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T6" s="76"/>
       <c r="U6" s="76"/>
-    </row>
-    <row r="7" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V6" s="76"/>
+    </row>
+    <row r="7" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="12">
         <v>1</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="79"/>
+      <c r="C7" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D7" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="15">
+      <c r="H7" s="15">
         <v>14</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="15">
+      <c r="K7" s="15">
         <v>20</v>
       </c>
-      <c r="K7" s="15">
+      <c r="L7" s="15">
         <v>240</v>
       </c>
-      <c r="L7" s="17" t="s">
+      <c r="M7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52" t="s">
+      <c r="N7" s="52"/>
+      <c r="O7" s="52" t="s">
         <v>214</v>
       </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="34" t="s">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="19">
+      <c r="S7" s="19">
         <v>3</v>
       </c>
-      <c r="S7" s="75" t="s">
+      <c r="T7" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T7" s="76"/>
       <c r="U7" s="76"/>
-    </row>
-    <row r="8" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V7" s="76"/>
+    </row>
+    <row r="8" spans="1:23" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="12">
         <v>1</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="79"/>
+      <c r="C8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D8" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="15">
+      <c r="F8" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="15">
         <v>18</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="J8" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="15">
+      <c r="K8" s="15">
         <v>20</v>
       </c>
-      <c r="K8" s="15">
+      <c r="L8" s="15">
         <v>180</v>
       </c>
-      <c r="L8" s="53" t="s">
+      <c r="M8" s="53" t="s">
         <v>246</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="65" t="s">
+      <c r="P8" s="2"/>
+      <c r="Q8" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="R8" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="R8" s="19">
+      <c r="S8" s="19">
         <v>1</v>
       </c>
-      <c r="S8" s="75" t="s">
+      <c r="T8" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T8" s="76"/>
       <c r="U8" s="76"/>
-    </row>
-    <row r="9" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V8" s="76"/>
+    </row>
+    <row r="9" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12">
         <v>1</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="D9" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="15">
+      <c r="H9" s="15">
         <v>20</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="J9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="K9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="15">
+      <c r="L9" s="15">
         <v>240</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="M9" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="17" t="s">
+      <c r="P9" s="2"/>
+      <c r="Q9" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="Q9" s="15" t="s">
+      <c r="R9" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="R9" s="19">
+      <c r="S9" s="19">
         <v>3</v>
       </c>
-      <c r="S9" s="75" t="s">
+      <c r="T9" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T9" s="76"/>
       <c r="U9" s="76"/>
-    </row>
-    <row r="10" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V9" s="76"/>
+    </row>
+    <row r="10" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="12">
         <v>1</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="79"/>
+      <c r="C10" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D10" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="19">
+      <c r="H10" s="19">
         <v>14</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="J10" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="15">
+      <c r="K10" s="15">
         <v>20</v>
       </c>
-      <c r="K10" s="15">
+      <c r="L10" s="15">
         <v>120</v>
       </c>
-      <c r="L10" s="17" t="s">
+      <c r="M10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52" t="s">
+      <c r="N10" s="52"/>
+      <c r="O10" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="Q10" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="R10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="R10" s="19">
+      <c r="S10" s="19">
         <v>3</v>
       </c>
-      <c r="S10" s="75" t="s">
+      <c r="T10" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T10" s="76"/>
       <c r="U10" s="76"/>
-    </row>
-    <row r="11" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V10" s="76"/>
+    </row>
+    <row r="11" spans="1:23" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
         <v>9</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="79"/>
+      <c r="C11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E11" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="15">
+      <c r="H11" s="15">
         <v>16</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="45" t="s">
+      <c r="J11" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="K11" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="K11" s="15">
+      <c r="L11" s="15">
         <v>105</v>
       </c>
-      <c r="L11" s="53" t="s">
+      <c r="M11" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="2"/>
+      <c r="P11" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="P11" s="59" t="s">
+      <c r="Q11" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="Q11" s="56" t="s">
+      <c r="R11" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="R11" s="19" t="s">
+      <c r="S11" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="S11" s="75" t="s">
+      <c r="T11" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T11" s="76"/>
       <c r="U11" s="76"/>
-    </row>
-    <row r="12" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V11" s="76"/>
+    </row>
+    <row r="12" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
         <v>1</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="79"/>
+      <c r="C12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="15">
+      <c r="H12" s="15">
         <v>14</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="I12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="J12" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="15">
+      <c r="K12" s="15">
         <v>20</v>
       </c>
-      <c r="K12" s="15">
+      <c r="L12" s="15">
         <v>360</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="M12" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52" t="s">
+      <c r="N12" s="52"/>
+      <c r="O12" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="19" t="s">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="R12" s="19">
+      <c r="S12" s="19">
         <v>3</v>
       </c>
-      <c r="S12" s="75" t="s">
+      <c r="T12" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T12" s="76"/>
       <c r="U12" s="76"/>
-    </row>
-    <row r="13" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V12" s="76"/>
+    </row>
+    <row r="13" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12">
         <v>1</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="79"/>
+      <c r="C13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="E13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H13" s="15">
         <v>14</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="I13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="J13" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="15">
         <v>30</v>
       </c>
-      <c r="K13" s="15">
+      <c r="L13" s="15">
         <v>240</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="M13" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52" t="s">
+      <c r="N13" s="52"/>
+      <c r="O13" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="O13" s="2"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="19" t="s">
+      <c r="P13" s="2"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="R13" s="19">
+      <c r="S13" s="19">
         <v>3</v>
       </c>
-      <c r="S13" s="75" t="s">
+      <c r="T13" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T13" s="76"/>
       <c r="U13" s="76"/>
-    </row>
-    <row r="14" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V13" s="76"/>
+    </row>
+    <row r="14" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="12">
         <v>1</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="79"/>
+      <c r="C14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="E14" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="15">
+      <c r="H14" s="15">
         <v>14</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="I14" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="J14" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="15">
+      <c r="K14" s="15">
         <v>30</v>
       </c>
-      <c r="K14" s="15">
+      <c r="L14" s="15">
         <v>360</v>
       </c>
-      <c r="L14" s="63" t="s">
+      <c r="M14" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52" t="s">
+      <c r="N14" s="52"/>
+      <c r="O14" s="52" t="s">
         <v>218</v>
       </c>
-      <c r="O14" s="2"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="19" t="s">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="R14" s="19">
+      <c r="S14" s="19">
         <v>3</v>
       </c>
-      <c r="S14" s="75" t="s">
+      <c r="T14" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T14" s="76"/>
       <c r="U14" s="76"/>
-    </row>
-    <row r="15" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V14" s="76"/>
+    </row>
+    <row r="15" spans="1:23" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="12">
         <v>2</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="79"/>
+      <c r="C15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E15" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="15">
+      <c r="H15" s="15">
         <v>8</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="I15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="J15" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="K15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="15">
+      <c r="L15" s="15">
         <v>120</v>
       </c>
-      <c r="L15" s="53" t="s">
+      <c r="M15" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="52" t="s">
+      <c r="N15" s="2"/>
+      <c r="O15" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="66" t="s">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="Q15" s="19" t="s">
+      <c r="R15" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="19">
+      <c r="S15" s="19">
         <v>2</v>
       </c>
-      <c r="S15" s="75" t="s">
+      <c r="T15" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T15" s="76"/>
       <c r="U15" s="76"/>
-      <c r="V15" s="75"/>
-    </row>
-    <row r="16" spans="1:22" ht="293.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V15" s="76"/>
+      <c r="W15" s="75"/>
+    </row>
+    <row r="16" spans="1:23" ht="293.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="12">
         <v>2</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="79"/>
+      <c r="C16" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="15">
+      <c r="H16" s="15">
         <v>8</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="I16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="J16" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="K16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="15">
+      <c r="L16" s="15">
         <v>120</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="M16" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="2"/>
+      <c r="O16" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="O16" s="2"/>
-      <c r="P16" s="69" t="s">
+      <c r="P16" s="2"/>
+      <c r="Q16" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="Q16" s="15" t="s">
+      <c r="R16" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="R16" s="19">
+      <c r="S16" s="19">
         <v>1</v>
       </c>
-      <c r="S16" s="75" t="s">
+      <c r="T16" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T16" s="76"/>
       <c r="U16" s="76"/>
-    </row>
-    <row r="17" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V16" s="76"/>
+    </row>
+    <row r="17" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="25">
         <v>3</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="81"/>
+      <c r="C17" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="15">
+      <c r="H17" s="15">
         <v>34</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="I17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="J17" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="K17" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="K17" s="15">
+      <c r="L17" s="15">
         <v>180</v>
       </c>
-      <c r="L17" s="17" t="s">
+      <c r="M17" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="19" t="s">
+      <c r="P17" s="2"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="R17" s="19">
+      <c r="S17" s="19">
         <v>1</v>
       </c>
-      <c r="S17" s="75" t="s">
+      <c r="T17" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T17" s="76"/>
       <c r="U17" s="76"/>
-    </row>
-    <row r="18" spans="1:21" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V17" s="76"/>
+    </row>
+    <row r="18" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12">
         <v>3</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="79"/>
+      <c r="C18" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="15">
+      <c r="H18" s="15">
         <v>34</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="I18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="J18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="K18" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="K18" s="15">
+      <c r="L18" s="15">
         <v>150</v>
       </c>
-      <c r="L18" s="53" t="s">
+      <c r="M18" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="2"/>
+      <c r="O18" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="O18" s="2"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="19" t="s">
+      <c r="P18" s="2"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="R18" s="19">
+      <c r="S18" s="19">
         <v>1</v>
       </c>
-      <c r="S18" s="75" t="s">
+      <c r="T18" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T18" s="76"/>
       <c r="U18" s="76"/>
-    </row>
-    <row r="19" spans="1:21" ht="303" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V18" s="76"/>
+    </row>
+    <row r="19" spans="1:22" ht="303" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="12">
         <v>3</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="79"/>
+      <c r="C19" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="15">
+      <c r="H19" s="15">
         <v>34</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="I19" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="J19" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="K19" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="K19" s="19">
+      <c r="L19" s="19">
         <v>180</v>
       </c>
-      <c r="L19" s="53" t="s">
+      <c r="M19" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="O19" s="2"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="56" t="s">
+      <c r="P19" s="2"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="R19" s="19">
+      <c r="S19" s="19">
         <v>1</v>
       </c>
-      <c r="S19" s="75" t="s">
+      <c r="T19" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T19" s="76"/>
       <c r="U19" s="76"/>
-    </row>
-    <row r="20" spans="1:21" ht="108" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V19" s="76"/>
+    </row>
+    <row r="20" spans="1:22" ht="108" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="12">
         <v>3</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="79"/>
+      <c r="C20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>20</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="15">
+      <c r="H20" s="15">
         <v>34</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="I20" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="J20" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="J20" s="15">
+      <c r="K20" s="15">
         <v>0.79500000000000004</v>
       </c>
-      <c r="K20" s="19">
+      <c r="L20" s="19">
         <v>60</v>
       </c>
-      <c r="L20" s="65" t="s">
+      <c r="M20" s="65" t="s">
         <v>226</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="66" t="s">
+      <c r="P20" s="2"/>
+      <c r="Q20" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="Q20" s="19" t="s">
+      <c r="R20" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="R20" s="19">
+      <c r="S20" s="19">
         <v>2</v>
       </c>
-      <c r="S20" s="75" t="s">
+      <c r="T20" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T20" s="76"/>
       <c r="U20" s="76"/>
-    </row>
-    <row r="21" spans="1:21" ht="274.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V20" s="76"/>
+    </row>
+    <row r="21" spans="1:22" ht="274.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="25">
         <v>5</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="81"/>
+      <c r="C21" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="D21" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E21" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="G21" s="28">
+      <c r="H21" s="28">
         <v>16</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="I21" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="I21" s="67" t="s">
+      <c r="J21" s="67" t="s">
         <v>125</v>
       </c>
-      <c r="J21" s="28">
+      <c r="K21" s="28">
         <v>14</v>
       </c>
-      <c r="K21" s="28">
+      <c r="L21" s="28">
         <v>85</v>
       </c>
-      <c r="L21" s="68" t="s">
+      <c r="M21" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="67" t="s">
+      <c r="P21" s="2"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="67" t="s">
         <v>234</v>
       </c>
-      <c r="R21" s="19">
+      <c r="S21" s="19">
         <v>1</v>
       </c>
-      <c r="S21" s="75" t="s">
+      <c r="T21" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T21" s="76"/>
       <c r="U21" s="76"/>
-    </row>
-    <row r="22" spans="1:21" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V21" s="76"/>
+    </row>
+    <row r="22" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
         <v>6</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="79"/>
+      <c r="C22" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="15">
+      <c r="H22" s="15">
         <v>8</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="I22" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I22" s="55" t="s">
+      <c r="J22" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="K22" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="15">
+      <c r="L22" s="15">
         <v>140</v>
       </c>
-      <c r="L22" s="17" t="s">
+      <c r="M22" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="P22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="P22" s="18" t="s">
+      <c r="Q22" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="Q22" s="19" t="s">
+      <c r="R22" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="R22" s="19">
+      <c r="S22" s="19">
         <v>2</v>
       </c>
-      <c r="S22" s="75" t="s">
+      <c r="T22" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T22" s="76"/>
       <c r="U22" s="76"/>
-    </row>
-    <row r="23" spans="1:21" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V22" s="76"/>
+    </row>
+    <row r="23" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12">
         <v>6</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="79"/>
+      <c r="C23" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E23" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G23" s="15">
+      <c r="H23" s="15">
         <v>8</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="I23" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="55" t="s">
+      <c r="J23" s="55" t="s">
         <v>220</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="K23" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="K23" s="15">
+      <c r="L23" s="15">
         <v>140</v>
       </c>
-      <c r="L23" s="14" t="s">
+      <c r="M23" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="2"/>
+      <c r="O23" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O23" s="2" t="s">
+      <c r="P23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="P23" s="50" t="s">
+      <c r="Q23" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="Q23" s="19" t="s">
+      <c r="R23" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="R23" s="19">
+      <c r="S23" s="19">
         <v>2</v>
       </c>
-      <c r="S23" s="75" t="s">
+      <c r="T23" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T23" s="76"/>
       <c r="U23" s="76"/>
-    </row>
-    <row r="24" spans="1:21" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V23" s="76"/>
+    </row>
+    <row r="24" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12">
         <v>6</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="79"/>
+      <c r="C24" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E24" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="G24" s="15">
+      <c r="H24" s="15">
         <v>8</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="I24" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I24" s="55" t="s">
+      <c r="J24" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="K24" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="15">
+      <c r="L24" s="15">
         <v>140</v>
       </c>
-      <c r="L24" s="17" t="s">
+      <c r="M24" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="2"/>
+      <c r="O24" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="P24" s="18" t="s">
+      <c r="Q24" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="Q24" s="56" t="s">
+      <c r="R24" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="R24" s="19">
+      <c r="S24" s="19">
         <v>2</v>
       </c>
-      <c r="S24" s="75" t="s">
+      <c r="T24" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T24" s="76"/>
       <c r="U24" s="76"/>
-    </row>
-    <row r="25" spans="1:21" ht="243" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V24" s="76"/>
+    </row>
+    <row r="25" spans="1:22" ht="243" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="12">
         <v>7</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="79"/>
+      <c r="C25" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="D25" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E25" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="15">
-        <v>17</v>
-      </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="15">
+        <v>17</v>
+      </c>
+      <c r="I25" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="J25" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="K25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="K25" s="15">
+      <c r="L25" s="15">
         <v>120</v>
       </c>
-      <c r="L25" s="53" t="s">
+      <c r="M25" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2" t="s">
+      <c r="N25" s="2"/>
+      <c r="O25" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="O25" s="2" t="s">
+      <c r="P25" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="56" t="s">
+      <c r="Q25" s="18"/>
+      <c r="R25" s="56" t="s">
         <v>232</v>
       </c>
-      <c r="R25" s="19">
+      <c r="S25" s="19">
         <v>3</v>
       </c>
-      <c r="S25" s="75" t="s">
+      <c r="T25" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T25" s="76"/>
       <c r="U25" s="76"/>
-    </row>
-    <row r="26" spans="1:21" ht="168" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V25" s="76"/>
+    </row>
+    <row r="26" spans="1:22" ht="168" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="12">
         <v>8</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="79"/>
+      <c r="C26" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E26" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="G26" s="15">
+      <c r="H26" s="15">
         <v>16</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="I26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="45" t="s">
+      <c r="J26" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="K26" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="K26" s="15">
+      <c r="L26" s="15">
         <v>85</v>
       </c>
-      <c r="L26" s="70" t="s">
+      <c r="M26" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="O26" s="2"/>
-      <c r="P26" s="14" t="s">
+      <c r="P26" s="2"/>
+      <c r="Q26" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="Q26" s="19" t="s">
+      <c r="R26" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="R26" s="19">
+      <c r="S26" s="19">
         <v>2</v>
       </c>
-      <c r="S26" s="75" t="s">
+      <c r="T26" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T26" s="76"/>
       <c r="U26" s="76"/>
-    </row>
-    <row r="27" spans="1:21" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V26" s="76"/>
+    </row>
+    <row r="27" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="33">
         <v>9</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="79"/>
+      <c r="C27" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E27" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="15">
+      <c r="H27" s="15">
         <v>16</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="I27" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="I27" s="45" t="s">
+      <c r="J27" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="K27" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="K27" s="15">
+      <c r="L27" s="15">
         <v>105</v>
       </c>
-      <c r="L27" s="53" t="s">
+      <c r="M27" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="M27" s="2"/>
       <c r="N27" s="2"/>
-      <c r="O27" s="2" t="s">
+      <c r="O27" s="2"/>
+      <c r="P27" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="P27" s="58" t="s">
+      <c r="Q27" s="58" t="s">
         <v>162</v>
       </c>
-      <c r="Q27" s="19" t="s">
+      <c r="R27" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="R27" s="19" t="s">
+      <c r="S27" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="S27" s="75" t="s">
+      <c r="T27" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T27" s="76"/>
       <c r="U27" s="76"/>
-    </row>
-    <row r="28" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V27" s="76"/>
+    </row>
+    <row r="28" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="12">
         <v>10</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="79"/>
+      <c r="C28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="D28" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E28" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="G28" s="15">
+      <c r="H28" s="15">
         <v>12</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="I28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="J28" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="J28" s="15" t="s">
+      <c r="K28" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="K28" s="15">
+      <c r="L28" s="15">
         <v>100</v>
       </c>
-      <c r="L28" s="53" t="s">
+      <c r="M28" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2" t="s">
+      <c r="N28" s="2"/>
+      <c r="O28" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="O28" s="2"/>
-      <c r="P28" s="43" t="s">
+      <c r="P28" s="2"/>
+      <c r="Q28" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="Q28" s="71" t="s">
+      <c r="R28" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="R28" s="19">
+      <c r="S28" s="19">
         <v>2</v>
       </c>
-      <c r="S28" s="75" t="s">
+      <c r="T28" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T28" s="76"/>
       <c r="U28" s="76"/>
-    </row>
-    <row r="29" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V28" s="76"/>
+    </row>
+    <row r="29" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="12">
         <v>10</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="79"/>
+      <c r="C29" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="D29" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E29" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="G29" s="36">
+      <c r="H29" s="36">
         <v>12</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="I29" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="46" t="s">
+      <c r="J29" s="46" t="s">
         <v>172</v>
       </c>
-      <c r="J29" s="36" t="s">
+      <c r="K29" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="K29" s="36">
+      <c r="L29" s="36">
         <v>360</v>
       </c>
-      <c r="L29" s="63" t="s">
+      <c r="M29" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2" t="s">
+      <c r="N29" s="2"/>
+      <c r="O29" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="O29" s="2"/>
-      <c r="P29" s="37" t="s">
+      <c r="P29" s="2"/>
+      <c r="Q29" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="Q29" s="71" t="s">
+      <c r="R29" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="R29" s="19">
+      <c r="S29" s="19">
         <v>2</v>
       </c>
-      <c r="S29" s="75" t="s">
+      <c r="T29" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T29" s="76"/>
       <c r="U29" s="76"/>
-    </row>
-    <row r="30" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V29" s="76"/>
+    </row>
+    <row r="30" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="12">
         <v>10</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="79"/>
+      <c r="C30" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="D30" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E30" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F30" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="G30" s="21">
+      <c r="H30" s="21">
         <v>12</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="I30" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="J30" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="K30" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="K30" s="21">
+      <c r="L30" s="21">
         <v>100</v>
       </c>
-      <c r="L30" s="37" t="s">
+      <c r="M30" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2" t="s">
+      <c r="N30" s="2"/>
+      <c r="O30" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="O30" s="2"/>
-      <c r="P30" s="38" t="s">
+      <c r="P30" s="2"/>
+      <c r="Q30" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="Q30" s="71" t="s">
+      <c r="R30" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="R30" s="19">
+      <c r="S30" s="19">
         <v>2</v>
       </c>
-      <c r="S30" s="75" t="s">
+      <c r="T30" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T30" s="76"/>
       <c r="U30" s="76"/>
-    </row>
-    <row r="31" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V30" s="76"/>
+    </row>
+    <row r="31" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="12">
         <v>10</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="79"/>
+      <c r="C31" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="D31" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E31" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="38" t="s">
+      <c r="F31" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="G31" s="21">
+      <c r="H31" s="21">
         <v>12</v>
       </c>
-      <c r="H31" s="15" t="s">
+      <c r="I31" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="J31" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="J31" s="21" t="s">
+      <c r="K31" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="K31" s="21">
+      <c r="L31" s="21">
         <v>360</v>
       </c>
-      <c r="L31" s="37" t="s">
+      <c r="M31" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2" t="s">
+      <c r="N31" s="2"/>
+      <c r="O31" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="O31" s="2"/>
-      <c r="P31" s="38" t="s">
+      <c r="P31" s="2"/>
+      <c r="Q31" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="Q31" s="71" t="s">
+      <c r="R31" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="R31" s="19">
+      <c r="S31" s="19">
         <v>2</v>
       </c>
-      <c r="S31" s="75" t="s">
+      <c r="T31" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T31" s="76"/>
       <c r="U31" s="76"/>
-    </row>
-    <row r="32" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V31" s="76"/>
+    </row>
+    <row r="32" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="12">
         <v>11</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="79"/>
+      <c r="C32" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="D32" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F32" s="38" t="s">
+      <c r="F32" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="G32" s="34">
+      <c r="H32" s="34">
         <v>40</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="I32" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="39" t="s">
+      <c r="J32" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="K32" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="K32" s="34">
+      <c r="L32" s="34">
         <v>90</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="M32" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2" t="s">
+      <c r="N32" s="2"/>
+      <c r="O32" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="O32" s="2" t="s">
+      <c r="P32" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="P32" s="41" t="s">
+      <c r="Q32" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="Q32" s="57" t="s">
+      <c r="R32" s="57" t="s">
         <v>233</v>
       </c>
-      <c r="R32" s="19">
+      <c r="S32" s="19">
         <v>1</v>
       </c>
-      <c r="S32" s="75" t="s">
+      <c r="T32" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T32" s="76"/>
       <c r="U32" s="76"/>
-    </row>
-    <row r="33" spans="1:21" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V32" s="76"/>
+    </row>
+    <row r="33" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="12">
         <v>12</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="79"/>
+      <c r="C33" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E33" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="41"/>
-      <c r="G33" s="21">
+      <c r="F33" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="41"/>
+      <c r="H33" s="21">
         <v>19</v>
       </c>
-      <c r="H33" s="21" t="s">
+      <c r="I33" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="I33" s="40" t="s">
+      <c r="J33" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="J33" s="21">
+      <c r="K33" s="21">
         <v>15</v>
       </c>
-      <c r="K33" s="21">
+      <c r="L33" s="21">
         <v>225</v>
       </c>
-      <c r="L33" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2" t="s">
+      <c r="N33" s="2"/>
+      <c r="O33" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="O33" s="2"/>
-      <c r="P33" s="48" t="s">
+      <c r="P33" s="2"/>
+      <c r="Q33" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="Q33" s="71" t="s">
+      <c r="R33" s="71" t="s">
         <v>237</v>
       </c>
-      <c r="R33" s="19">
+      <c r="S33" s="19">
         <v>2</v>
       </c>
-      <c r="S33" s="75" t="s">
+      <c r="T33" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T33" s="76"/>
       <c r="U33" s="76"/>
-    </row>
-    <row r="34" spans="1:21" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V33" s="76"/>
+    </row>
+    <row r="34" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="12">
         <v>12</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="79"/>
+      <c r="C34" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="D34" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E34" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="38" t="s">
+      <c r="F34" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="G34" s="21">
+      <c r="H34" s="21">
         <v>19</v>
       </c>
-      <c r="H34" s="21" t="s">
+      <c r="I34" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="40" t="s">
+      <c r="J34" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="J34" s="21">
+      <c r="K34" s="21">
         <v>15</v>
       </c>
-      <c r="K34" s="21">
+      <c r="L34" s="21">
         <v>172</v>
       </c>
-      <c r="L34" s="3" t="s">
+      <c r="M34" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="62" t="s">
+      <c r="P34" s="2"/>
+      <c r="Q34" s="62" t="s">
         <v>195</v>
       </c>
-      <c r="Q34" s="34"/>
-      <c r="R34" s="19">
+      <c r="R34" s="34"/>
+      <c r="S34" s="19">
         <v>3</v>
       </c>
-      <c r="S34" s="75" t="s">
+      <c r="T34" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T34" s="76"/>
       <c r="U34" s="76"/>
-    </row>
-    <row r="35" spans="1:21" ht="231.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V34" s="76"/>
+    </row>
+    <row r="35" spans="1:22" ht="231.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="12">
         <v>12</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="79"/>
+      <c r="C35" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="D35" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E35" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="38" t="s">
+      <c r="F35" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="G35" s="21">
+      <c r="H35" s="21">
         <v>21</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="I35" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="I35" s="40" t="s">
+      <c r="J35" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="J35" s="21">
+      <c r="K35" s="21">
         <v>15</v>
       </c>
-      <c r="K35" s="21">
+      <c r="L35" s="21">
         <v>153</v>
       </c>
-      <c r="L35" s="49" t="s">
+      <c r="M35" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="M35" s="2" t="s">
+      <c r="N35" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="3" t="s">
+      <c r="P35" s="2"/>
+      <c r="Q35" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="Q35" s="34"/>
-      <c r="R35" s="19">
+      <c r="R35" s="34"/>
+      <c r="S35" s="19">
         <v>3</v>
       </c>
-      <c r="S35" s="75" t="s">
+      <c r="T35" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T35" s="76"/>
       <c r="U35" s="76"/>
-    </row>
-    <row r="36" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V35" s="76"/>
+    </row>
+    <row r="36" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A36" s="12">
         <v>12</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="79"/>
+      <c r="C36" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="D36" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="63" t="s">
-        <v>17</v>
-      </c>
       <c r="E36" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="38" t="s">
+      <c r="F36" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="G36" s="21">
+      <c r="H36" s="21">
         <v>21</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="I36" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="I36" s="40" t="s">
+      <c r="J36" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J36" s="21">
+      <c r="K36" s="21">
         <v>15</v>
       </c>
-      <c r="K36" s="21">
+      <c r="L36" s="21">
         <v>166</v>
       </c>
-      <c r="L36" s="37" t="s">
+      <c r="M36" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="M36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="19">
+      <c r="P36" s="2"/>
+      <c r="Q36" s="48"/>
+      <c r="R36" s="34"/>
+      <c r="S36" s="19">
         <v>2</v>
       </c>
-      <c r="S36" s="75" t="s">
+      <c r="T36" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T36" s="76"/>
       <c r="U36" s="76"/>
-    </row>
-    <row r="37" spans="1:21" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V36" s="76"/>
+    </row>
+    <row r="37" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" s="12">
         <v>1</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="79"/>
+      <c r="C37" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="D37" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="41"/>
-      <c r="G37" s="21">
+      <c r="F37" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="41"/>
+      <c r="H37" s="21">
         <v>18</v>
       </c>
-      <c r="H37" s="21" t="s">
+      <c r="I37" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I37" s="40" t="s">
+      <c r="J37" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="21">
+      <c r="K37" s="21">
         <v>30</v>
       </c>
-      <c r="K37" s="21">
+      <c r="L37" s="21">
         <v>180</v>
       </c>
-      <c r="L37" s="3" t="s">
+      <c r="M37" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="N37" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="65" t="s">
+      <c r="P37" s="2"/>
+      <c r="Q37" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="Q37" s="19" t="s">
+      <c r="R37" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="R37" s="19">
+      <c r="S37" s="19">
         <v>1</v>
       </c>
-      <c r="S37" s="75" t="s">
+      <c r="T37" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T37" s="76"/>
       <c r="U37" s="76"/>
-    </row>
-    <row r="38" spans="1:21" ht="276" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V37" s="76"/>
+    </row>
+    <row r="38" spans="1:22" ht="276" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="33">
         <v>1</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="79"/>
+      <c r="C38" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="21" t="s">
+      <c r="D38" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="E38" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="38" t="s">
+      <c r="F38" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="21">
+      <c r="H38" s="21">
         <v>20</v>
       </c>
-      <c r="H38" s="21" t="s">
+      <c r="I38" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="I38" s="40" t="s">
+      <c r="J38" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J38" s="21">
+      <c r="K38" s="21">
         <v>30</v>
       </c>
-      <c r="K38" s="21">
+      <c r="L38" s="21">
         <v>240</v>
       </c>
-      <c r="L38" s="48" t="s">
+      <c r="M38" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="N38" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="78" t="s">
+      <c r="P38" s="2"/>
+      <c r="Q38" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="Q38" s="21" t="s">
+      <c r="R38" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="R38" s="19">
+      <c r="S38" s="19">
         <v>3</v>
       </c>
-      <c r="S38" s="75" t="s">
+      <c r="T38" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T38" s="76"/>
       <c r="U38" s="76"/>
-    </row>
-    <row r="39" spans="1:21" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V38" s="76"/>
+    </row>
+    <row r="39" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="42">
         <v>1</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="79"/>
+      <c r="C39" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="D39" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="E39" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="38" t="s">
+      <c r="F39" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="34">
+      <c r="H39" s="34">
         <v>14</v>
       </c>
-      <c r="H39" s="21" t="s">
+      <c r="I39" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="40" t="s">
+      <c r="J39" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="J39" s="21">
+      <c r="K39" s="21">
         <v>30</v>
       </c>
-      <c r="K39" s="21">
+      <c r="L39" s="21">
         <v>120</v>
       </c>
-      <c r="L39" s="37" t="s">
+      <c r="M39" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52" t="s">
+      <c r="N39" s="52"/>
+      <c r="O39" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="P39" s="78" t="s">
+      <c r="Q39" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="Q39" s="34" t="s">
+      <c r="R39" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="R39" s="19">
+      <c r="S39" s="19">
         <v>3</v>
       </c>
-      <c r="S39" s="75" t="s">
+      <c r="T39" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T39" s="76"/>
       <c r="U39" s="76"/>
-    </row>
-    <row r="40" spans="1:21" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V39" s="76"/>
+    </row>
+    <row r="40" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="42">
         <v>6</v>
       </c>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="79"/>
+      <c r="C40" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="D40" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="43" t="s">
+      <c r="F40" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="G40" s="44">
+      <c r="H40" s="44">
         <v>8</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="I40" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I40" s="40" t="s">
+      <c r="J40" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="J40" s="21" t="s">
+      <c r="K40" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="K40" s="21">
+      <c r="L40" s="21">
         <v>140</v>
       </c>
-      <c r="L40" s="15" t="s">
+      <c r="M40" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2" t="s">
+      <c r="N40" s="2"/>
+      <c r="O40" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="O40" s="2" t="s">
+      <c r="P40" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P40" s="48" t="s">
+      <c r="Q40" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="Q40" s="57" t="s">
+      <c r="R40" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="R40" s="19">
+      <c r="S40" s="19">
         <v>2</v>
       </c>
-      <c r="S40" s="75" t="s">
+      <c r="T40" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T40" s="76"/>
       <c r="U40" s="76"/>
-    </row>
-    <row r="41" spans="1:21" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V40" s="76"/>
+    </row>
+    <row r="41" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="42">
         <v>9</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="79"/>
+      <c r="C41" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="D41" s="21" t="s">
         <v>32</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="E41" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="43" t="s">
+      <c r="F41" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G41" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="44">
+      <c r="H41" s="44">
         <v>16</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="I41" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I41" s="61" t="s">
+      <c r="J41" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="J41" s="21" t="s">
+      <c r="K41" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="K41" s="21">
+      <c r="L41" s="21">
         <v>105</v>
       </c>
-      <c r="L41" s="3" t="s">
+      <c r="M41" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2" t="s">
+      <c r="N41" s="2"/>
+      <c r="O41" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="P41" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P41" s="60" t="s">
+      <c r="Q41" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="Q41" s="57" t="s">
+      <c r="R41" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="R41" s="19">
+      <c r="S41" s="19">
         <v>2</v>
       </c>
-      <c r="S41" s="75" t="s">
+      <c r="T41" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T41" s="76"/>
       <c r="U41" s="76"/>
-    </row>
-    <row r="42" spans="1:21" ht="186.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="V41" s="76"/>
+    </row>
+    <row r="42" spans="1:22" ht="186.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="79">
         <v>13</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="79"/>
+      <c r="C42" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="D42" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="D42" s="21" t="s">
-        <v>17</v>
-      </c>
       <c r="E42" s="21" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="G42" s="21">
+      <c r="H42" s="21">
         <v>25</v>
       </c>
-      <c r="H42" s="21" t="s">
+      <c r="I42" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21">
+      <c r="J42" s="21"/>
+      <c r="K42" s="21">
         <v>17.5</v>
       </c>
-      <c r="K42" s="21">
+      <c r="L42" s="21">
         <v>80</v>
       </c>
-      <c r="L42" s="71" t="s">
+      <c r="M42" s="71" t="s">
         <v>266</v>
       </c>
-      <c r="M42" s="21">
+      <c r="N42" s="21">
         <v>1.75</v>
       </c>
-      <c r="N42" s="21"/>
       <c r="O42" s="21"/>
       <c r="P42" s="21"/>
-      <c r="Q42" s="21" t="s">
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="R42" s="21"/>
-      <c r="S42" s="75" t="s">
+      <c r="S42" s="21"/>
+      <c r="T42" s="75" t="s">
         <v>255</v>
       </c>
-      <c r="T42" s="21"/>
       <c r="U42" s="21"/>
+      <c r="V42" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U42" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
-  <conditionalFormatting sqref="M19">
+  <autoFilter ref="A1:V42" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
+  <conditionalFormatting sqref="N19">
     <cfRule type="duplicateValues" dxfId="35" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20">
+  <conditionalFormatting sqref="N20">
     <cfRule type="duplicateValues" dxfId="34" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M21:M41 M1:M18 M43:M1048576">
+  <conditionalFormatting sqref="N21:N41 N1:N18 N43:N1048576">
     <cfRule type="duplicateValues" dxfId="33" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4">
+  <conditionalFormatting sqref="O4">
     <cfRule type="duplicateValues" dxfId="32" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="O5">
     <cfRule type="duplicateValues" dxfId="31" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N6">
+  <conditionalFormatting sqref="O6">
     <cfRule type="duplicateValues" dxfId="30" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N7">
+  <conditionalFormatting sqref="O7">
     <cfRule type="duplicateValues" dxfId="29" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N10">
+  <conditionalFormatting sqref="O10">
     <cfRule type="duplicateValues" dxfId="28" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N12">
+  <conditionalFormatting sqref="O12">
     <cfRule type="duplicateValues" dxfId="27" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13">
+  <conditionalFormatting sqref="O13">
     <cfRule type="duplicateValues" dxfId="26" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14">
+  <conditionalFormatting sqref="O14">
     <cfRule type="duplicateValues" dxfId="25" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N39">
+  <conditionalFormatting sqref="O39">
     <cfRule type="duplicateValues" dxfId="24" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O25">
+  <conditionalFormatting sqref="P25">
     <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O32">
+  <conditionalFormatting sqref="P32">
     <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
udpated EF fir ID 13 in ACC
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34B272F0-9865-4FE5-8ECE-D5905CF8D327}"/>
+  <xr:revisionPtr revIDLastSave="637" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DCC559D-C3F5-47F0-A458-212C7FF60D02}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="271">
   <si>
     <t>CognitiveFunction</t>
   </si>
@@ -2082,6 +2082,9 @@
   </si>
   <si>
     <t>Timepoint</t>
+  </si>
+  <si>
+    <t>-1.34</t>
   </si>
 </sst>
 </file>
@@ -3331,8 +3334,8 @@
   <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5254,7 +5257,7 @@
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2" t="s">
-        <v>238</v>
+        <v>270</v>
       </c>
       <c r="P33" s="2"/>
       <c r="Q33" s="48" t="s">

</xml_diff>

<commit_message>
double checked sec to ms
</commit_message>
<xml_diff>
--- a/Overview_Studies.xlsx
+++ b/Overview_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f2d186216cf91ab/Bidlung/University/M.S. Leiden University/M.S. Neuroscience (Research)/Internship Groningen/GitHub_Multiverse_meta/MetaAnalysis-Psilo-Cognition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="678" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69DF6B97-1B2C-4888-894E-EDC136C21F93}"/>
+  <xr:revisionPtr revIDLastSave="681" documentId="13_ncr:1_{525082E2-B509-430B-A115-E19A7741069F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2339B3C2-3B33-472D-B6D8-ACF2315A27AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1725" yWindow="-17835" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -3331,11 +3331,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3544,7 +3545,7 @@
       <c r="U3" s="76"/>
       <c r="V3" s="76"/>
     </row>
-    <row r="4" spans="1:23" ht="321.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23" ht="321.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -3606,7 +3607,7 @@
       <c r="U4" s="76"/>
       <c r="V4" s="76"/>
     </row>
-    <row r="5" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -3664,7 +3665,7 @@
       <c r="U5" s="76"/>
       <c r="V5" s="76"/>
     </row>
-    <row r="6" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="12">
         <v>1</v>
       </c>
@@ -3722,7 +3723,7 @@
       <c r="U6" s="76"/>
       <c r="V6" s="76"/>
     </row>
-    <row r="7" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="12">
         <v>1</v>
       </c>
@@ -3898,7 +3899,7 @@
       <c r="U9" s="76"/>
       <c r="V9" s="76"/>
     </row>
-    <row r="10" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="12">
         <v>1</v>
       </c>
@@ -3960,7 +3961,7 @@
       <c r="U10" s="76"/>
       <c r="V10" s="76"/>
     </row>
-    <row r="11" spans="1:23" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:23" ht="409.6" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -4020,7 +4021,7 @@
       <c r="U11" s="76"/>
       <c r="V11" s="76"/>
     </row>
-    <row r="12" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12">
         <v>1</v>
       </c>
@@ -4078,7 +4079,7 @@
       <c r="U12" s="76"/>
       <c r="V12" s="76"/>
     </row>
-    <row r="13" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="12">
         <v>1</v>
       </c>
@@ -4136,7 +4137,7 @@
       <c r="U13" s="76"/>
       <c r="V13" s="76"/>
     </row>
-    <row r="14" spans="1:23" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:23" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="12">
         <v>1</v>
       </c>
@@ -4194,7 +4195,7 @@
       <c r="U14" s="76"/>
       <c r="V14" s="76"/>
     </row>
-    <row r="15" spans="1:23" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:23" ht="409.6" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="12">
         <v>2</v>
       </c>
@@ -4255,7 +4256,7 @@
       <c r="V15" s="76"/>
       <c r="W15" s="75"/>
     </row>
-    <row r="16" spans="1:23" ht="293.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:23" ht="293.25" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="12">
         <v>2</v>
       </c>
@@ -4375,7 +4376,7 @@
       <c r="U17" s="76"/>
       <c r="V17" s="76"/>
     </row>
-    <row r="18" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" ht="288.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="12">
         <v>3</v>
       </c>
@@ -4611,7 +4612,7 @@
       <c r="U21" s="76"/>
       <c r="V21" s="76"/>
     </row>
-    <row r="22" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:22" ht="288.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="12">
         <v>6</v>
       </c>
@@ -4673,7 +4674,7 @@
       <c r="U22" s="76"/>
       <c r="V22" s="76"/>
     </row>
-    <row r="23" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:22" ht="288.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="12">
         <v>6</v>
       </c>
@@ -4735,7 +4736,7 @@
       <c r="U23" s="76"/>
       <c r="V23" s="76"/>
     </row>
-    <row r="24" spans="1:22" ht="288.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" ht="288.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="12">
         <v>6</v>
       </c>
@@ -4797,7 +4798,7 @@
       <c r="U24" s="76"/>
       <c r="V24" s="76"/>
     </row>
-    <row r="25" spans="1:22" ht="243" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:22" ht="243" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="12">
         <v>7</v>
       </c>
@@ -4919,7 +4920,7 @@
       <c r="U26" s="76"/>
       <c r="V26" s="76"/>
     </row>
-    <row r="27" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:22" ht="409.6" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="33">
         <v>9</v>
       </c>
@@ -4979,7 +4980,7 @@
       <c r="U27" s="76"/>
       <c r="V27" s="76"/>
     </row>
-    <row r="28" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:22" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="12">
         <v>10</v>
       </c>
@@ -5039,7 +5040,7 @@
       <c r="U28" s="76"/>
       <c r="V28" s="76"/>
     </row>
-    <row r="29" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:22" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="12">
         <v>10</v>
       </c>
@@ -5099,7 +5100,7 @@
       <c r="U29" s="76"/>
       <c r="V29" s="76"/>
     </row>
-    <row r="30" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:22" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="12">
         <v>10</v>
       </c>
@@ -5159,7 +5160,7 @@
       <c r="U30" s="76"/>
       <c r="V30" s="76"/>
     </row>
-    <row r="31" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="12">
         <v>10</v>
       </c>
@@ -5219,7 +5220,7 @@
       <c r="U31" s="76"/>
       <c r="V31" s="76"/>
     </row>
-    <row r="32" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:22" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="12">
         <v>11</v>
       </c>
@@ -5281,7 +5282,7 @@
       <c r="U32" s="76"/>
       <c r="V32" s="76"/>
     </row>
-    <row r="33" spans="1:22" ht="160.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:22" ht="160.5" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="12">
         <v>12</v>
       </c>
@@ -5629,7 +5630,7 @@
       <c r="U38" s="76"/>
       <c r="V38" s="76"/>
     </row>
-    <row r="39" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:22" ht="409.6" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="42">
         <v>1</v>
       </c>
@@ -5691,7 +5692,7 @@
       <c r="U39" s="76"/>
       <c r="V39" s="76"/>
     </row>
-    <row r="40" spans="1:22" ht="105.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:22" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="42">
         <v>6</v>
       </c>
@@ -5753,7 +5754,7 @@
       <c r="U40" s="76"/>
       <c r="V40" s="76"/>
     </row>
-    <row r="41" spans="1:22" ht="409.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:22" ht="409.6" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="42">
         <v>9</v>
       </c>
@@ -5870,7 +5871,27 @@
       <c r="V42" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V42" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}"/>
+  <autoFilter ref="A1:V42" xr:uid="{2EF2F6BA-3E86-4A09-A91D-773D5C504DD4}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+        <filter val="16"/>
+        <filter val="18"/>
+        <filter val="19"/>
+        <filter val="2"/>
+        <filter val="20"/>
+        <filter val="25"/>
+        <filter val="33"/>
+        <filter val="34"/>
+        <filter val="35"/>
+        <filter val="36"/>
+        <filter val="37"/>
+        <filter val="41"/>
+        <filter val="7"/>
+        <filter val="8"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="N19">
     <cfRule type="duplicateValues" dxfId="35" priority="14"/>
   </conditionalFormatting>

</xml_diff>